<commit_message>
update data and guide
</commit_message>
<xml_diff>
--- a/experimental_context_description.xlsx
+++ b/experimental_context_description.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vignevin-my.sharepoint.com/personal/xavier_delpuech_vignevin_com/Documents/AgricultureNumerique/ProjetsEnCours/VITISDATACROP/05_TRAVAIL_EN_COURS/WP1.1 Harmonisation/Expérimentation/vitisdatacrop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xdelpuech\OneDrive - vignevin.com\AgricultureNumerique\ProjetsEnCours\VITISDATACROP\05_TRAVAIL_EN_COURS\WP1.1 Harmonisation\Expérimentation\vitisdatacrop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="529" documentId="8_{F5B98E63-5745-4FF3-8CEE-474CD3F71BC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B03E6CE-4DB8-4CE0-8FE7-B0498197B608}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32B7449F-90EF-4F9B-8AB1-EA4CC5B47857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1AE09EEA-C0A3-42DC-AFC7-BA79A75A8C50}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{1AE09EEA-C0A3-42DC-AFC7-BA79A75A8C50}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="399">
   <si>
     <t>experimentation</t>
   </si>
@@ -1230,6 +1230,18 @@
   </si>
   <si>
     <t>A</t>
+  </si>
+  <si>
+    <t>subplot_trt</t>
+  </si>
+  <si>
+    <t>Traitement</t>
+  </si>
+  <si>
+    <t>Code du traitement appliqué sur la placette</t>
+  </si>
+  <si>
+    <t>TEM</t>
   </si>
 </sst>
 </file>
@@ -1331,10 +1343,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1634,23 +1642,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB13ADFC-DCBE-45B8-93DC-72D8CCE37DD2}">
-  <dimension ref="A1:T94"/>
+  <dimension ref="A1:T95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H94" sqref="H94"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E86" sqref="E86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="101.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="101.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>11</v>
       </c>
@@ -1712,1733 +1720,1733 @@
         <v>233</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>281</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>282</v>
       </c>
       <c r="C2" t="s">
-        <v>144</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>140</v>
+        <v>284</v>
+      </c>
+      <c r="D2" t="s">
+        <v>285</v>
+      </c>
+      <c r="E2" t="s">
+        <v>287</v>
       </c>
       <c r="F2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>281</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>283</v>
       </c>
       <c r="C3" t="s">
-        <v>145</v>
+        <v>286</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>139</v>
+        <v>288</v>
+      </c>
+      <c r="E3" t="s">
+        <v>289</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3" t="s">
-        <v>21</v>
-      </c>
-      <c r="T3" s="6" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>202</v>
       </c>
       <c r="B4" t="s">
-        <v>147</v>
+        <v>203</v>
       </c>
       <c r="C4" t="s">
-        <v>146</v>
+        <v>204</v>
       </c>
       <c r="D4" t="s">
-        <v>154</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>138</v>
+        <v>211</v>
+      </c>
+      <c r="E4" t="s">
+        <v>217</v>
       </c>
       <c r="F4" t="s">
-        <v>20</v>
-      </c>
-      <c r="K4" t="s">
-        <v>21</v>
-      </c>
-      <c r="T4" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>0</v>
+        <v>202</v>
       </c>
       <c r="B5" t="s">
-        <v>148</v>
+        <v>225</v>
       </c>
       <c r="C5" t="s">
-        <v>125</v>
+        <v>205</v>
       </c>
       <c r="D5" t="s">
-        <v>120</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>132</v>
+        <v>212</v>
+      </c>
+      <c r="E5" t="s">
+        <v>218</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
       </c>
-      <c r="G5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>0</v>
+        <v>202</v>
       </c>
       <c r="B6" t="s">
-        <v>149</v>
+        <v>224</v>
       </c>
       <c r="C6" t="s">
-        <v>126</v>
+        <v>206</v>
       </c>
       <c r="D6" t="s">
-        <v>121</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>133</v>
+        <v>213</v>
+      </c>
+      <c r="E6" t="s">
+        <v>219</v>
       </c>
       <c r="F6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="J6" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>0</v>
+        <v>202</v>
       </c>
       <c r="B7" t="s">
-        <v>152</v>
+        <v>226</v>
       </c>
       <c r="C7" t="s">
-        <v>127</v>
+        <v>207</v>
       </c>
       <c r="D7" t="s">
-        <v>155</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>137</v>
+        <v>214</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
       </c>
       <c r="F7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>0</v>
+        <v>202</v>
       </c>
       <c r="B8" t="s">
-        <v>153</v>
+        <v>227</v>
       </c>
       <c r="C8" t="s">
-        <v>128</v>
+        <v>208</v>
       </c>
       <c r="D8" t="s">
-        <v>122</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>134</v>
+        <v>215</v>
+      </c>
+      <c r="E8">
+        <v>215</v>
       </c>
       <c r="F8" t="s">
-        <v>141</v>
-      </c>
-      <c r="G8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>0</v>
+        <v>202</v>
       </c>
       <c r="B9" t="s">
-        <v>150</v>
+        <v>228</v>
       </c>
       <c r="C9" t="s">
-        <v>130</v>
+        <v>209</v>
       </c>
       <c r="D9" t="s">
-        <v>131</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>135</v>
+        <v>223</v>
+      </c>
+      <c r="E9" t="s">
+        <v>220</v>
       </c>
       <c r="F9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>0</v>
+        <v>202</v>
       </c>
       <c r="B10" t="s">
-        <v>151</v>
+        <v>229</v>
       </c>
       <c r="C10" t="s">
-        <v>129</v>
+        <v>210</v>
       </c>
       <c r="D10" t="s">
-        <v>124</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>136</v>
+        <v>216</v>
+      </c>
+      <c r="E10" t="s">
+        <v>221</v>
       </c>
       <c r="F10" t="s">
         <v>13</v>
       </c>
-      <c r="N10" t="s">
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>202</v>
+      </c>
+      <c r="B11" t="s">
+        <v>242</v>
+      </c>
+      <c r="C11" t="s">
+        <v>239</v>
+      </c>
+      <c r="D11" t="s">
+        <v>240</v>
+      </c>
+      <c r="E11" t="s">
+        <v>241</v>
+      </c>
+      <c r="F11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>202</v>
+      </c>
+      <c r="B12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C12" t="s">
+        <v>243</v>
+      </c>
+      <c r="D12" t="s">
+        <v>253</v>
+      </c>
+      <c r="E12" t="s">
+        <v>263</v>
+      </c>
+      <c r="F12" t="s">
+        <v>270</v>
+      </c>
+      <c r="J12" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>202</v>
+      </c>
+      <c r="B13" t="s">
+        <v>273</v>
+      </c>
+      <c r="C13" t="s">
+        <v>244</v>
+      </c>
+      <c r="D13" t="s">
+        <v>254</v>
+      </c>
+      <c r="E13" t="s">
+        <v>264</v>
+      </c>
+      <c r="F13" t="s">
+        <v>270</v>
+      </c>
+      <c r="J13" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>202</v>
+      </c>
+      <c r="B14" t="s">
+        <v>272</v>
+      </c>
+      <c r="C14" t="s">
+        <v>245</v>
+      </c>
+      <c r="D14" t="s">
+        <v>255</v>
+      </c>
+      <c r="E14" t="s">
+        <v>263</v>
+      </c>
+      <c r="F14" t="s">
+        <v>270</v>
+      </c>
+      <c r="J14" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>202</v>
+      </c>
+      <c r="B15" t="s">
+        <v>276</v>
+      </c>
+      <c r="C15" t="s">
+        <v>246</v>
+      </c>
+      <c r="D15" t="s">
+        <v>256</v>
+      </c>
+      <c r="E15" t="s">
+        <v>263</v>
+      </c>
+      <c r="F15" t="s">
+        <v>270</v>
+      </c>
+      <c r="J15" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>202</v>
+      </c>
+      <c r="B16" t="s">
+        <v>277</v>
+      </c>
+      <c r="C16" t="s">
+        <v>247</v>
+      </c>
+      <c r="D16" t="s">
+        <v>257</v>
+      </c>
+      <c r="E16" t="s">
+        <v>264</v>
+      </c>
+      <c r="F16" t="s">
+        <v>270</v>
+      </c>
+      <c r="J16" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>202</v>
+      </c>
+      <c r="B17" t="s">
+        <v>274</v>
+      </c>
+      <c r="C17" t="s">
+        <v>248</v>
+      </c>
+      <c r="D17" t="s">
+        <v>258</v>
+      </c>
+      <c r="E17" t="s">
+        <v>263</v>
+      </c>
+      <c r="F17" t="s">
+        <v>270</v>
+      </c>
+      <c r="J17" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>202</v>
+      </c>
+      <c r="B18" t="s">
+        <v>278</v>
+      </c>
+      <c r="C18" t="s">
+        <v>249</v>
+      </c>
+      <c r="D18" t="s">
+        <v>259</v>
+      </c>
+      <c r="E18" t="s">
+        <v>264</v>
+      </c>
+      <c r="F18" t="s">
+        <v>270</v>
+      </c>
+      <c r="J18" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>202</v>
+      </c>
+      <c r="B19" t="s">
+        <v>275</v>
+      </c>
+      <c r="C19" t="s">
+        <v>250</v>
+      </c>
+      <c r="D19" t="s">
+        <v>260</v>
+      </c>
+      <c r="E19" t="s">
+        <v>264</v>
+      </c>
+      <c r="F19" t="s">
+        <v>270</v>
+      </c>
+      <c r="J19" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>202</v>
+      </c>
+      <c r="B20" t="s">
+        <v>279</v>
+      </c>
+      <c r="C20" t="s">
+        <v>251</v>
+      </c>
+      <c r="D20" t="s">
+        <v>261</v>
+      </c>
+      <c r="E20" t="s">
+        <v>263</v>
+      </c>
+      <c r="F20" t="s">
+        <v>270</v>
+      </c>
+      <c r="J20" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>202</v>
+      </c>
+      <c r="B21" t="s">
+        <v>280</v>
+      </c>
+      <c r="C21" t="s">
+        <v>252</v>
+      </c>
+      <c r="D21" t="s">
+        <v>262</v>
+      </c>
+      <c r="E21" t="s">
+        <v>263</v>
+      </c>
+      <c r="F21" t="s">
+        <v>270</v>
+      </c>
+      <c r="J21" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" t="s">
+        <v>144</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F22" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" t="s">
+        <v>145</v>
+      </c>
+      <c r="D23" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="F23" t="s">
+        <v>20</v>
+      </c>
+      <c r="G23" t="s">
+        <v>17</v>
+      </c>
+      <c r="K23" t="s">
+        <v>21</v>
+      </c>
+      <c r="T23" s="6" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" t="s">
+        <v>147</v>
+      </c>
+      <c r="C24" t="s">
+        <v>146</v>
+      </c>
+      <c r="D24" t="s">
+        <v>154</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F24" t="s">
+        <v>20</v>
+      </c>
+      <c r="K24" t="s">
+        <v>21</v>
+      </c>
+      <c r="T24" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" t="s">
+        <v>148</v>
+      </c>
+      <c r="C25" t="s">
+        <v>125</v>
+      </c>
+      <c r="D25" t="s">
+        <v>120</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" t="s">
+        <v>149</v>
+      </c>
+      <c r="C26" t="s">
+        <v>126</v>
+      </c>
+      <c r="D26" t="s">
+        <v>121</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" t="s">
+        <v>152</v>
+      </c>
+      <c r="C27" t="s">
+        <v>127</v>
+      </c>
+      <c r="D27" t="s">
+        <v>155</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F27" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" t="s">
+        <v>153</v>
+      </c>
+      <c r="C28" t="s">
+        <v>128</v>
+      </c>
+      <c r="D28" t="s">
+        <v>122</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="F28" t="s">
+        <v>141</v>
+      </c>
+      <c r="G28" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" t="s">
+        <v>150</v>
+      </c>
+      <c r="C29" t="s">
+        <v>130</v>
+      </c>
+      <c r="D29" t="s">
+        <v>131</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F29" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" t="s">
+        <v>151</v>
+      </c>
+      <c r="C30" t="s">
+        <v>129</v>
+      </c>
+      <c r="D30" t="s">
+        <v>124</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="F30" t="s">
+        <v>13</v>
+      </c>
+      <c r="N30" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" t="s">
-        <v>142</v>
-      </c>
-      <c r="D11" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11">
-        <v>43.692996999999998</v>
-      </c>
-      <c r="F11" t="s">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>156</v>
+      </c>
+      <c r="B31" t="s">
+        <v>169</v>
+      </c>
+      <c r="C31" t="s">
+        <v>157</v>
+      </c>
+      <c r="D31" t="s">
+        <v>163</v>
+      </c>
+      <c r="E31">
+        <v>2010</v>
+      </c>
+      <c r="F31" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>156</v>
+      </c>
+      <c r="B32" t="s">
+        <v>170</v>
+      </c>
+      <c r="C32" t="s">
+        <v>158</v>
+      </c>
+      <c r="D32" t="s">
+        <v>164</v>
+      </c>
+      <c r="E32">
+        <v>50</v>
+      </c>
+      <c r="F32" t="s">
         <v>23</v>
       </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>90</v>
-      </c>
-      <c r="K11" t="s">
-        <v>24</v>
-      </c>
-      <c r="O11">
-        <v>43.692996999999998</v>
-      </c>
-      <c r="T11" s="5" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" t="s">
-        <v>143</v>
-      </c>
-      <c r="D12" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12">
-        <v>4.2784149999999999</v>
-      </c>
-      <c r="F12" t="s">
-        <v>23</v>
-      </c>
-      <c r="H12">
-        <v>-180</v>
-      </c>
-      <c r="I12">
-        <v>180</v>
-      </c>
-      <c r="K12" t="s">
-        <v>25</v>
-      </c>
-      <c r="O12">
-        <v>4.2784149999999999</v>
-      </c>
-      <c r="T12" s="3" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" t="s">
-        <v>33</v>
-      </c>
-      <c r="E13" t="s">
-        <v>34</v>
-      </c>
-      <c r="F13" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13" t="s">
-        <v>17</v>
-      </c>
-      <c r="S13" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" t="s">
-        <v>44</v>
-      </c>
-      <c r="E14" t="s">
-        <v>45</v>
-      </c>
-      <c r="F14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" t="s">
-        <v>46</v>
-      </c>
-      <c r="C15" t="s">
-        <v>47</v>
-      </c>
-      <c r="D15" t="s">
-        <v>48</v>
-      </c>
-      <c r="E15" t="s">
-        <v>51</v>
-      </c>
-      <c r="F15" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q15" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" t="s">
-        <v>268</v>
-      </c>
-      <c r="C16" t="s">
-        <v>267</v>
-      </c>
-      <c r="D16" t="s">
-        <v>266</v>
-      </c>
-      <c r="E16">
-        <v>30341</v>
-      </c>
-      <c r="F16" t="s">
-        <v>13</v>
-      </c>
-      <c r="L16" t="s">
-        <v>269</v>
-      </c>
-      <c r="Q16" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" t="s">
-        <v>52</v>
-      </c>
-      <c r="C17" t="s">
-        <v>53</v>
-      </c>
-      <c r="D17" t="s">
-        <v>54</v>
-      </c>
-      <c r="E17" t="s">
-        <v>55</v>
-      </c>
-      <c r="F17" t="s">
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>156</v>
+      </c>
+      <c r="B33" t="s">
+        <v>172</v>
+      </c>
+      <c r="C33" t="s">
+        <v>159</v>
+      </c>
+      <c r="D33" t="s">
+        <v>165</v>
+      </c>
+      <c r="E33">
         <v>30</v>
-      </c>
-      <c r="J17" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" t="s">
-        <v>57</v>
-      </c>
-      <c r="C18" t="s">
-        <v>58</v>
-      </c>
-      <c r="D18" t="s">
-        <v>59</v>
-      </c>
-      <c r="E18">
-        <v>1998</v>
-      </c>
-      <c r="F18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" t="s">
-        <v>61</v>
-      </c>
-      <c r="C19" t="s">
-        <v>62</v>
-      </c>
-      <c r="D19" t="s">
-        <v>63</v>
-      </c>
-      <c r="E19" t="s">
-        <v>64</v>
-      </c>
-      <c r="F19" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" t="s">
-        <v>65</v>
-      </c>
-      <c r="C20" t="s">
-        <v>66</v>
-      </c>
-      <c r="D20" t="s">
-        <v>71</v>
-      </c>
-      <c r="E20" t="s">
-        <v>67</v>
-      </c>
-      <c r="F20" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" t="s">
-        <v>68</v>
-      </c>
-      <c r="C21" t="s">
-        <v>69</v>
-      </c>
-      <c r="D21" t="s">
-        <v>70</v>
-      </c>
-      <c r="E21" t="s">
-        <v>72</v>
-      </c>
-      <c r="F21" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" t="s">
-        <v>93</v>
-      </c>
-      <c r="C22" t="s">
-        <v>73</v>
-      </c>
-      <c r="D22" t="s">
-        <v>74</v>
-      </c>
-      <c r="E22">
-        <v>2.5</v>
-      </c>
-      <c r="F22" t="s">
-        <v>23</v>
-      </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>94</v>
-      </c>
-      <c r="C23" t="s">
-        <v>81</v>
-      </c>
-      <c r="D23" t="s">
-        <v>75</v>
-      </c>
-      <c r="E23">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="F23" t="s">
-        <v>23</v>
-      </c>
-      <c r="H23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>22</v>
-      </c>
-      <c r="B24" t="s">
-        <v>91</v>
-      </c>
-      <c r="C24" t="s">
-        <v>82</v>
-      </c>
-      <c r="D24" t="s">
-        <v>108</v>
-      </c>
-      <c r="E24" t="s">
-        <v>102</v>
-      </c>
-      <c r="F24" t="s">
-        <v>30</v>
-      </c>
-      <c r="J24" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>22</v>
-      </c>
-      <c r="B25" t="s">
-        <v>92</v>
-      </c>
-      <c r="C25" t="s">
-        <v>83</v>
-      </c>
-      <c r="D25" t="s">
-        <v>109</v>
-      </c>
-      <c r="E25" t="s">
-        <v>103</v>
-      </c>
-      <c r="F25" t="s">
-        <v>30</v>
-      </c>
-      <c r="J25" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>22</v>
-      </c>
-      <c r="B26" t="s">
-        <v>39</v>
-      </c>
-      <c r="C26" t="s">
-        <v>26</v>
-      </c>
-      <c r="D26" t="s">
-        <v>29</v>
-      </c>
-      <c r="E26" t="s">
-        <v>32</v>
-      </c>
-      <c r="F26" t="s">
-        <v>30</v>
-      </c>
-      <c r="J26" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>22</v>
-      </c>
-      <c r="B27" t="s">
-        <v>95</v>
-      </c>
-      <c r="C27" t="s">
-        <v>84</v>
-      </c>
-      <c r="D27" t="s">
-        <v>76</v>
-      </c>
-      <c r="E27">
-        <v>93</v>
-      </c>
-      <c r="F27" t="s">
-        <v>23</v>
-      </c>
-      <c r="H27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>22</v>
-      </c>
-      <c r="B28" t="s">
-        <v>96</v>
-      </c>
-      <c r="C28" t="s">
-        <v>85</v>
-      </c>
-      <c r="D28" t="s">
-        <v>110</v>
-      </c>
-      <c r="E28" t="s">
-        <v>104</v>
-      </c>
-      <c r="F28" t="s">
-        <v>30</v>
-      </c>
-      <c r="J28" t="s">
-        <v>113</v>
-      </c>
-      <c r="P28" t="s">
-        <v>118</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>111</v>
-      </c>
-      <c r="T28" s="3" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>22</v>
-      </c>
-      <c r="B29" t="s">
-        <v>97</v>
-      </c>
-      <c r="C29" t="s">
-        <v>86</v>
-      </c>
-      <c r="D29" t="s">
-        <v>77</v>
-      </c>
-      <c r="E29" t="s">
-        <v>105</v>
-      </c>
-      <c r="F29" t="s">
-        <v>30</v>
-      </c>
-      <c r="J29" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>22</v>
-      </c>
-      <c r="B30" t="s">
-        <v>98</v>
-      </c>
-      <c r="C30" t="s">
-        <v>87</v>
-      </c>
-      <c r="D30" t="s">
-        <v>78</v>
-      </c>
-      <c r="E30" t="s">
-        <v>105</v>
-      </c>
-      <c r="F30" t="s">
-        <v>30</v>
-      </c>
-      <c r="J30" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>22</v>
-      </c>
-      <c r="B31" t="s">
-        <v>99</v>
-      </c>
-      <c r="C31" t="s">
-        <v>88</v>
-      </c>
-      <c r="D31" t="s">
-        <v>79</v>
-      </c>
-      <c r="E31" t="s">
-        <v>106</v>
-      </c>
-      <c r="F31" t="s">
-        <v>30</v>
-      </c>
-      <c r="J31" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>22</v>
-      </c>
-      <c r="B32" t="s">
-        <v>100</v>
-      </c>
-      <c r="C32" t="s">
-        <v>89</v>
-      </c>
-      <c r="D32" t="s">
-        <v>80</v>
-      </c>
-      <c r="E32" t="s">
-        <v>107</v>
-      </c>
-      <c r="F32" t="s">
-        <v>30</v>
-      </c>
-      <c r="J32" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>22</v>
-      </c>
-      <c r="B33" t="s">
-        <v>101</v>
-      </c>
-      <c r="C33" t="s">
-        <v>90</v>
-      </c>
-      <c r="D33" t="s">
-        <v>119</v>
-      </c>
-      <c r="E33">
-        <v>3.5</v>
       </c>
       <c r="F33" t="s">
         <v>23</v>
       </c>
-      <c r="H33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>156</v>
       </c>
       <c r="B34" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C34" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="D34" t="s">
-        <v>163</v>
-      </c>
-      <c r="E34">
-        <v>2010</v>
+        <v>166</v>
+      </c>
+      <c r="E34" t="s">
+        <v>175</v>
       </c>
       <c r="F34" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="J34" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>156</v>
       </c>
       <c r="B35" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="C35" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="D35" t="s">
-        <v>164</v>
-      </c>
-      <c r="E35">
-        <v>50</v>
+        <v>167</v>
+      </c>
+      <c r="E35" t="s">
+        <v>176</v>
       </c>
       <c r="F35" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>156</v>
       </c>
       <c r="B36" t="s">
-        <v>172</v>
+        <v>340</v>
       </c>
       <c r="C36" t="s">
-        <v>159</v>
+        <v>341</v>
       </c>
       <c r="D36" t="s">
-        <v>165</v>
-      </c>
-      <c r="E36">
+        <v>342</v>
+      </c>
+      <c r="E36" t="s">
+        <v>343</v>
+      </c>
+      <c r="F36" t="s">
         <v>30</v>
       </c>
-      <c r="F36" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="J36" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>156</v>
       </c>
       <c r="B37" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="C37" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D37" t="s">
-        <v>166</v>
-      </c>
-      <c r="E37" t="s">
-        <v>175</v>
+        <v>168</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
       </c>
       <c r="F37" t="s">
-        <v>30</v>
-      </c>
-      <c r="J37" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>156</v>
+        <v>22</v>
       </c>
       <c r="B38" t="s">
-        <v>173</v>
+        <v>40</v>
       </c>
       <c r="C38" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="D38" t="s">
-        <v>167</v>
-      </c>
-      <c r="E38" t="s">
-        <v>176</v>
+        <v>27</v>
+      </c>
+      <c r="E38">
+        <v>43.692996999999998</v>
       </c>
       <c r="F38" t="s">
+        <v>23</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <v>90</v>
+      </c>
+      <c r="K38" t="s">
+        <v>24</v>
+      </c>
+      <c r="O38">
+        <v>43.692996999999998</v>
+      </c>
+      <c r="T38" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>22</v>
+      </c>
+      <c r="B39" t="s">
+        <v>41</v>
+      </c>
+      <c r="C39" t="s">
+        <v>143</v>
+      </c>
+      <c r="D39" t="s">
+        <v>28</v>
+      </c>
+      <c r="E39">
+        <v>4.2784149999999999</v>
+      </c>
+      <c r="F39" t="s">
+        <v>23</v>
+      </c>
+      <c r="H39">
+        <v>-180</v>
+      </c>
+      <c r="I39">
+        <v>180</v>
+      </c>
+      <c r="K39" t="s">
+        <v>25</v>
+      </c>
+      <c r="O39">
+        <v>4.2784149999999999</v>
+      </c>
+      <c r="T39" s="3" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>22</v>
+      </c>
+      <c r="B40" t="s">
+        <v>35</v>
+      </c>
+      <c r="C40" t="s">
+        <v>43</v>
+      </c>
+      <c r="D40" t="s">
+        <v>33</v>
+      </c>
+      <c r="E40" t="s">
+        <v>34</v>
+      </c>
+      <c r="F40" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>156</v>
-      </c>
-      <c r="B39" t="s">
-        <v>340</v>
-      </c>
-      <c r="C39" t="s">
-        <v>341</v>
-      </c>
-      <c r="D39" t="s">
-        <v>342</v>
-      </c>
-      <c r="E39" t="s">
-        <v>343</v>
-      </c>
-      <c r="F39" t="s">
-        <v>30</v>
-      </c>
-      <c r="J39" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>156</v>
-      </c>
-      <c r="B40" t="s">
-        <v>174</v>
-      </c>
-      <c r="C40" t="s">
-        <v>162</v>
-      </c>
-      <c r="D40" t="s">
-        <v>168</v>
-      </c>
-      <c r="E40">
-        <v>0</v>
-      </c>
-      <c r="F40" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G40" t="s">
+        <v>17</v>
+      </c>
+      <c r="S40" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>178</v>
+        <v>22</v>
       </c>
       <c r="B41" t="s">
-        <v>189</v>
+        <v>36</v>
       </c>
       <c r="C41" t="s">
-        <v>179</v>
+        <v>42</v>
       </c>
       <c r="D41" t="s">
-        <v>185</v>
+        <v>44</v>
       </c>
       <c r="E41" t="s">
-        <v>197</v>
+        <v>45</v>
       </c>
       <c r="F41" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>178</v>
+        <v>22</v>
       </c>
       <c r="B42" t="s">
-        <v>191</v>
+        <v>46</v>
       </c>
       <c r="C42" t="s">
-        <v>180</v>
+        <v>47</v>
       </c>
       <c r="D42" t="s">
-        <v>333</v>
-      </c>
-      <c r="E42">
-        <v>1.5</v>
+        <v>48</v>
+      </c>
+      <c r="E42" t="s">
+        <v>51</v>
       </c>
       <c r="F42" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="Q42" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>178</v>
+        <v>22</v>
       </c>
       <c r="B43" t="s">
-        <v>190</v>
+        <v>268</v>
       </c>
       <c r="C43" t="s">
-        <v>181</v>
+        <v>267</v>
       </c>
       <c r="D43" t="s">
-        <v>195</v>
-      </c>
-      <c r="E43" t="s">
-        <v>198</v>
+        <v>266</v>
+      </c>
+      <c r="E43">
+        <v>30341</v>
       </c>
       <c r="F43" t="s">
-        <v>30</v>
-      </c>
-      <c r="J43" t="s">
-        <v>200</v>
-      </c>
-      <c r="Q43" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="L43" t="s">
+        <v>269</v>
+      </c>
+      <c r="Q43" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>178</v>
+        <v>22</v>
       </c>
       <c r="B44" t="s">
-        <v>192</v>
+        <v>52</v>
       </c>
       <c r="C44" t="s">
-        <v>182</v>
+        <v>53</v>
       </c>
       <c r="D44" t="s">
-        <v>186</v>
+        <v>54</v>
       </c>
       <c r="E44" t="s">
-        <v>199</v>
+        <v>55</v>
       </c>
       <c r="F44" t="s">
         <v>30</v>
       </c>
       <c r="J44" t="s">
-        <v>201</v>
-      </c>
-      <c r="P44" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>178</v>
+        <v>22</v>
       </c>
       <c r="B45" t="s">
-        <v>193</v>
+        <v>57</v>
       </c>
       <c r="C45" t="s">
-        <v>183</v>
+        <v>58</v>
       </c>
       <c r="D45" t="s">
-        <v>187</v>
+        <v>59</v>
       </c>
       <c r="E45">
-        <v>2</v>
+        <v>1998</v>
       </c>
       <c r="F45" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>178</v>
+        <v>22</v>
       </c>
       <c r="B46" t="s">
-        <v>194</v>
+        <v>61</v>
       </c>
       <c r="C46" t="s">
-        <v>184</v>
+        <v>62</v>
       </c>
       <c r="D46" t="s">
-        <v>188</v>
-      </c>
-      <c r="E46">
-        <v>6.5</v>
+        <v>63</v>
+      </c>
+      <c r="E46" t="s">
+        <v>64</v>
       </c>
       <c r="F46" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>202</v>
+        <v>22</v>
       </c>
       <c r="B47" t="s">
-        <v>203</v>
+        <v>65</v>
       </c>
       <c r="C47" t="s">
-        <v>204</v>
+        <v>66</v>
       </c>
       <c r="D47" t="s">
-        <v>211</v>
+        <v>71</v>
       </c>
       <c r="E47" t="s">
-        <v>217</v>
+        <v>67</v>
       </c>
       <c r="F47" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>202</v>
+        <v>22</v>
       </c>
       <c r="B48" t="s">
-        <v>225</v>
+        <v>68</v>
       </c>
       <c r="C48" t="s">
-        <v>205</v>
+        <v>69</v>
       </c>
       <c r="D48" t="s">
-        <v>212</v>
+        <v>70</v>
       </c>
       <c r="E48" t="s">
-        <v>218</v>
+        <v>72</v>
       </c>
       <c r="F48" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>202</v>
+        <v>22</v>
       </c>
       <c r="B49" t="s">
-        <v>224</v>
+        <v>93</v>
       </c>
       <c r="C49" t="s">
-        <v>206</v>
+        <v>73</v>
       </c>
       <c r="D49" t="s">
-        <v>213</v>
-      </c>
-      <c r="E49" t="s">
-        <v>219</v>
+        <v>74</v>
+      </c>
+      <c r="E49">
+        <v>2.5</v>
       </c>
       <c r="F49" t="s">
+        <v>23</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>22</v>
+      </c>
+      <c r="B50" t="s">
+        <v>94</v>
+      </c>
+      <c r="C50" t="s">
+        <v>81</v>
+      </c>
+      <c r="D50" t="s">
+        <v>75</v>
+      </c>
+      <c r="E50">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F50" t="s">
+        <v>23</v>
+      </c>
+      <c r="H50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>22</v>
+      </c>
+      <c r="B51" t="s">
+        <v>91</v>
+      </c>
+      <c r="C51" t="s">
+        <v>82</v>
+      </c>
+      <c r="D51" t="s">
+        <v>108</v>
+      </c>
+      <c r="E51" t="s">
+        <v>102</v>
+      </c>
+      <c r="F51" t="s">
         <v>30</v>
       </c>
-      <c r="J49" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>202</v>
-      </c>
-      <c r="B50" t="s">
-        <v>226</v>
-      </c>
-      <c r="C50" t="s">
-        <v>207</v>
-      </c>
-      <c r="D50" t="s">
-        <v>214</v>
-      </c>
-      <c r="E50">
-        <v>3</v>
-      </c>
-      <c r="F50" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>202</v>
-      </c>
-      <c r="B51" t="s">
-        <v>227</v>
-      </c>
-      <c r="C51" t="s">
-        <v>208</v>
-      </c>
-      <c r="D51" t="s">
-        <v>215</v>
-      </c>
-      <c r="E51">
-        <v>215</v>
-      </c>
-      <c r="F51" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J51" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>202</v>
+        <v>22</v>
       </c>
       <c r="B52" t="s">
-        <v>228</v>
+        <v>92</v>
       </c>
       <c r="C52" t="s">
-        <v>209</v>
+        <v>83</v>
       </c>
       <c r="D52" t="s">
-        <v>223</v>
+        <v>109</v>
       </c>
       <c r="E52" t="s">
-        <v>220</v>
+        <v>103</v>
       </c>
       <c r="F52" t="s">
+        <v>30</v>
+      </c>
+      <c r="J52" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>22</v>
+      </c>
+      <c r="B53" t="s">
+        <v>39</v>
+      </c>
+      <c r="C53" t="s">
+        <v>26</v>
+      </c>
+      <c r="D53" t="s">
+        <v>29</v>
+      </c>
+      <c r="E53" t="s">
+        <v>32</v>
+      </c>
+      <c r="F53" t="s">
+        <v>30</v>
+      </c>
+      <c r="J53" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>22</v>
+      </c>
+      <c r="B54" t="s">
+        <v>95</v>
+      </c>
+      <c r="C54" t="s">
+        <v>84</v>
+      </c>
+      <c r="D54" t="s">
+        <v>76</v>
+      </c>
+      <c r="E54">
+        <v>93</v>
+      </c>
+      <c r="F54" t="s">
+        <v>23</v>
+      </c>
+      <c r="H54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>22</v>
+      </c>
+      <c r="B55" t="s">
+        <v>96</v>
+      </c>
+      <c r="C55" t="s">
+        <v>85</v>
+      </c>
+      <c r="D55" t="s">
+        <v>110</v>
+      </c>
+      <c r="E55" t="s">
+        <v>104</v>
+      </c>
+      <c r="F55" t="s">
+        <v>30</v>
+      </c>
+      <c r="J55" t="s">
+        <v>113</v>
+      </c>
+      <c r="P55" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q55" t="s">
+        <v>111</v>
+      </c>
+      <c r="T55" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>22</v>
+      </c>
+      <c r="B56" t="s">
+        <v>97</v>
+      </c>
+      <c r="C56" t="s">
+        <v>86</v>
+      </c>
+      <c r="D56" t="s">
+        <v>77</v>
+      </c>
+      <c r="E56" t="s">
+        <v>105</v>
+      </c>
+      <c r="F56" t="s">
+        <v>30</v>
+      </c>
+      <c r="J56" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>22</v>
+      </c>
+      <c r="B57" t="s">
+        <v>98</v>
+      </c>
+      <c r="C57" t="s">
+        <v>87</v>
+      </c>
+      <c r="D57" t="s">
+        <v>78</v>
+      </c>
+      <c r="E57" t="s">
+        <v>105</v>
+      </c>
+      <c r="F57" t="s">
+        <v>30</v>
+      </c>
+      <c r="J57" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>22</v>
+      </c>
+      <c r="B58" t="s">
+        <v>99</v>
+      </c>
+      <c r="C58" t="s">
+        <v>88</v>
+      </c>
+      <c r="D58" t="s">
+        <v>79</v>
+      </c>
+      <c r="E58" t="s">
+        <v>106</v>
+      </c>
+      <c r="F58" t="s">
+        <v>30</v>
+      </c>
+      <c r="J58" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>22</v>
+      </c>
+      <c r="B59" t="s">
+        <v>100</v>
+      </c>
+      <c r="C59" t="s">
+        <v>89</v>
+      </c>
+      <c r="D59" t="s">
+        <v>80</v>
+      </c>
+      <c r="E59" t="s">
+        <v>107</v>
+      </c>
+      <c r="F59" t="s">
+        <v>30</v>
+      </c>
+      <c r="J59" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>22</v>
+      </c>
+      <c r="B60" t="s">
+        <v>101</v>
+      </c>
+      <c r="C60" t="s">
+        <v>90</v>
+      </c>
+      <c r="D60" t="s">
+        <v>119</v>
+      </c>
+      <c r="E60">
+        <v>3.5</v>
+      </c>
+      <c r="F60" t="s">
+        <v>23</v>
+      </c>
+      <c r="H60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>22</v>
+      </c>
+      <c r="B61" t="s">
+        <v>323</v>
+      </c>
+      <c r="C61" t="s">
+        <v>324</v>
+      </c>
+      <c r="D61" t="s">
+        <v>325</v>
+      </c>
+      <c r="E61">
+        <v>0.5</v>
+      </c>
+      <c r="F61" t="s">
+        <v>23</v>
+      </c>
+      <c r="H61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>22</v>
+      </c>
+      <c r="B62" t="s">
+        <v>326</v>
+      </c>
+      <c r="C62" t="s">
+        <v>327</v>
+      </c>
+      <c r="D62" t="s">
+        <v>328</v>
+      </c>
+      <c r="E62">
+        <v>3500</v>
+      </c>
+      <c r="F62" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>22</v>
+      </c>
+      <c r="B63" t="s">
+        <v>329</v>
+      </c>
+      <c r="C63" t="s">
+        <v>330</v>
+      </c>
+      <c r="D63" t="s">
+        <v>330</v>
+      </c>
+      <c r="E63" t="s">
+        <v>331</v>
+      </c>
+      <c r="F63" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>202</v>
-      </c>
-      <c r="B53" t="s">
-        <v>229</v>
-      </c>
-      <c r="C53" t="s">
-        <v>210</v>
-      </c>
-      <c r="D53" t="s">
-        <v>216</v>
-      </c>
-      <c r="E53" t="s">
-        <v>221</v>
-      </c>
-      <c r="F53" t="s">
+      <c r="J63" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>291</v>
+      </c>
+      <c r="B64" t="s">
+        <v>290</v>
+      </c>
+      <c r="C64" t="s">
+        <v>296</v>
+      </c>
+      <c r="D64" t="s">
+        <v>292</v>
+      </c>
+      <c r="E64" t="s">
+        <v>304</v>
+      </c>
+      <c r="F64" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>202</v>
-      </c>
-      <c r="B54" t="s">
-        <v>242</v>
-      </c>
-      <c r="C54" t="s">
-        <v>239</v>
-      </c>
-      <c r="D54" t="s">
-        <v>240</v>
-      </c>
-      <c r="E54" t="s">
-        <v>241</v>
-      </c>
-      <c r="F54" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>202</v>
-      </c>
-      <c r="B55" t="s">
-        <v>271</v>
-      </c>
-      <c r="C55" t="s">
-        <v>243</v>
-      </c>
-      <c r="D55" t="s">
-        <v>253</v>
-      </c>
-      <c r="E55" t="s">
-        <v>263</v>
-      </c>
-      <c r="F55" t="s">
-        <v>270</v>
-      </c>
-      <c r="J55" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>202</v>
-      </c>
-      <c r="B56" t="s">
-        <v>273</v>
-      </c>
-      <c r="C56" t="s">
-        <v>244</v>
-      </c>
-      <c r="D56" t="s">
-        <v>254</v>
-      </c>
-      <c r="E56" t="s">
-        <v>264</v>
-      </c>
-      <c r="F56" t="s">
-        <v>270</v>
-      </c>
-      <c r="J56" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>202</v>
-      </c>
-      <c r="B57" t="s">
-        <v>272</v>
-      </c>
-      <c r="C57" t="s">
-        <v>245</v>
-      </c>
-      <c r="D57" t="s">
-        <v>255</v>
-      </c>
-      <c r="E57" t="s">
-        <v>263</v>
-      </c>
-      <c r="F57" t="s">
-        <v>270</v>
-      </c>
-      <c r="J57" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>202</v>
-      </c>
-      <c r="B58" t="s">
-        <v>276</v>
-      </c>
-      <c r="C58" t="s">
-        <v>246</v>
-      </c>
-      <c r="D58" t="s">
-        <v>256</v>
-      </c>
-      <c r="E58" t="s">
-        <v>263</v>
-      </c>
-      <c r="F58" t="s">
-        <v>270</v>
-      </c>
-      <c r="J58" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>202</v>
-      </c>
-      <c r="B59" t="s">
-        <v>277</v>
-      </c>
-      <c r="C59" t="s">
-        <v>247</v>
-      </c>
-      <c r="D59" t="s">
-        <v>257</v>
-      </c>
-      <c r="E59" t="s">
-        <v>264</v>
-      </c>
-      <c r="F59" t="s">
-        <v>270</v>
-      </c>
-      <c r="J59" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>202</v>
-      </c>
-      <c r="B60" t="s">
-        <v>274</v>
-      </c>
-      <c r="C60" t="s">
-        <v>248</v>
-      </c>
-      <c r="D60" t="s">
-        <v>258</v>
-      </c>
-      <c r="E60" t="s">
-        <v>263</v>
-      </c>
-      <c r="F60" t="s">
-        <v>270</v>
-      </c>
-      <c r="J60" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>202</v>
-      </c>
-      <c r="B61" t="s">
-        <v>278</v>
-      </c>
-      <c r="C61" t="s">
-        <v>249</v>
-      </c>
-      <c r="D61" t="s">
-        <v>259</v>
-      </c>
-      <c r="E61" t="s">
-        <v>264</v>
-      </c>
-      <c r="F61" t="s">
-        <v>270</v>
-      </c>
-      <c r="J61" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>202</v>
-      </c>
-      <c r="B62" t="s">
-        <v>275</v>
-      </c>
-      <c r="C62" t="s">
-        <v>250</v>
-      </c>
-      <c r="D62" t="s">
-        <v>260</v>
-      </c>
-      <c r="E62" t="s">
-        <v>264</v>
-      </c>
-      <c r="F62" t="s">
-        <v>270</v>
-      </c>
-      <c r="J62" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>202</v>
-      </c>
-      <c r="B63" t="s">
-        <v>279</v>
-      </c>
-      <c r="C63" t="s">
-        <v>251</v>
-      </c>
-      <c r="D63" t="s">
-        <v>261</v>
-      </c>
-      <c r="E63" t="s">
-        <v>263</v>
-      </c>
-      <c r="F63" t="s">
-        <v>270</v>
-      </c>
-      <c r="J63" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>202</v>
-      </c>
-      <c r="B64" t="s">
-        <v>280</v>
-      </c>
-      <c r="C64" t="s">
-        <v>252</v>
-      </c>
-      <c r="D64" t="s">
-        <v>262</v>
-      </c>
-      <c r="E64" t="s">
-        <v>263</v>
-      </c>
-      <c r="F64" t="s">
-        <v>270</v>
-      </c>
-      <c r="J64" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>281</v>
+        <v>291</v>
       </c>
       <c r="B65" t="s">
-        <v>282</v>
+        <v>314</v>
       </c>
       <c r="C65" t="s">
-        <v>284</v>
+        <v>297</v>
       </c>
       <c r="D65" t="s">
-        <v>285</v>
+        <v>293</v>
       </c>
       <c r="E65" t="s">
-        <v>287</v>
+        <v>135</v>
       </c>
       <c r="F65" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>281</v>
+        <v>291</v>
       </c>
       <c r="B66" t="s">
-        <v>283</v>
+        <v>316</v>
       </c>
       <c r="C66" t="s">
-        <v>286</v>
+        <v>298</v>
       </c>
       <c r="D66" t="s">
-        <v>288</v>
+        <v>312</v>
       </c>
       <c r="E66" t="s">
-        <v>289</v>
+        <v>305</v>
       </c>
       <c r="F66" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="K66" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>291</v>
       </c>
       <c r="B67" t="s">
-        <v>290</v>
+        <v>317</v>
       </c>
       <c r="C67" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="D67" t="s">
-        <v>292</v>
+        <v>313</v>
       </c>
       <c r="E67" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="F67" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="K67" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>291</v>
       </c>
       <c r="B68" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="C68" t="s">
-        <v>297</v>
+        <v>125</v>
       </c>
       <c r="D68" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="E68" t="s">
-        <v>135</v>
+        <v>307</v>
       </c>
       <c r="F68" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>291</v>
       </c>
       <c r="B69" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="C69" t="s">
-        <v>298</v>
+        <v>126</v>
       </c>
       <c r="D69" t="s">
-        <v>312</v>
+        <v>295</v>
       </c>
       <c r="E69" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="F69" t="s">
-        <v>20</v>
-      </c>
-      <c r="K69" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>291</v>
       </c>
       <c r="B70" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="C70" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D70" t="s">
-        <v>313</v>
+        <v>322</v>
       </c>
       <c r="E70" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="F70" t="s">
-        <v>20</v>
-      </c>
-      <c r="K70" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>291</v>
       </c>
       <c r="B71" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="C71" t="s">
-        <v>125</v>
+        <v>301</v>
       </c>
       <c r="D71" t="s">
-        <v>294</v>
+        <v>122</v>
       </c>
       <c r="E71" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="F71" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>291</v>
       </c>
       <c r="B72" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="C72" t="s">
-        <v>126</v>
+        <v>302</v>
       </c>
       <c r="D72" t="s">
-        <v>295</v>
+        <v>303</v>
       </c>
       <c r="E72" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="F72" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>291</v>
+        <v>178</v>
       </c>
       <c r="B73" t="s">
-        <v>320</v>
+        <v>189</v>
       </c>
       <c r="C73" t="s">
-        <v>300</v>
+        <v>179</v>
       </c>
       <c r="D73" t="s">
-        <v>322</v>
+        <v>185</v>
       </c>
       <c r="E73" t="s">
-        <v>309</v>
+        <v>197</v>
       </c>
       <c r="F73" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>291</v>
+        <v>178</v>
       </c>
       <c r="B74" t="s">
-        <v>321</v>
+        <v>191</v>
       </c>
       <c r="C74" t="s">
-        <v>301</v>
+        <v>180</v>
       </c>
       <c r="D74" t="s">
-        <v>122</v>
-      </c>
-      <c r="E74" t="s">
-        <v>310</v>
+        <v>333</v>
+      </c>
+      <c r="E74">
+        <v>1.5</v>
       </c>
       <c r="F74" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>291</v>
+        <v>178</v>
       </c>
       <c r="B75" t="s">
-        <v>315</v>
+        <v>190</v>
       </c>
       <c r="C75" t="s">
-        <v>302</v>
+        <v>181</v>
       </c>
       <c r="D75" t="s">
-        <v>303</v>
+        <v>195</v>
       </c>
       <c r="E75" t="s">
-        <v>311</v>
+        <v>198</v>
       </c>
       <c r="F75" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="J75" t="s">
+        <v>200</v>
+      </c>
+      <c r="Q75" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>22</v>
+        <v>178</v>
       </c>
       <c r="B76" t="s">
-        <v>323</v>
+        <v>192</v>
       </c>
       <c r="C76" t="s">
-        <v>324</v>
+        <v>182</v>
       </c>
       <c r="D76" t="s">
-        <v>325</v>
-      </c>
-      <c r="E76">
-        <v>0.5</v>
+        <v>186</v>
+      </c>
+      <c r="E76" t="s">
+        <v>199</v>
       </c>
       <c r="F76" t="s">
-        <v>23</v>
-      </c>
-      <c r="H76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="J76" t="s">
+        <v>201</v>
+      </c>
+      <c r="P76" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>22</v>
+        <v>178</v>
       </c>
       <c r="B77" t="s">
-        <v>326</v>
+        <v>193</v>
       </c>
       <c r="C77" t="s">
-        <v>327</v>
+        <v>183</v>
       </c>
       <c r="D77" t="s">
-        <v>328</v>
+        <v>187</v>
       </c>
       <c r="E77">
-        <v>3500</v>
+        <v>2</v>
       </c>
       <c r="F77" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>22</v>
+        <v>178</v>
       </c>
       <c r="B78" t="s">
-        <v>329</v>
+        <v>194</v>
       </c>
       <c r="C78" t="s">
-        <v>330</v>
+        <v>184</v>
       </c>
       <c r="D78" t="s">
-        <v>330</v>
-      </c>
-      <c r="E78" t="s">
-        <v>331</v>
+        <v>188</v>
+      </c>
+      <c r="E78">
+        <v>6.5</v>
       </c>
       <c r="F78" t="s">
-        <v>13</v>
-      </c>
-      <c r="J78" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>178</v>
       </c>
@@ -3461,331 +3469,354 @@
         <v>338</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>345</v>
+        <v>379</v>
       </c>
       <c r="B80" t="s">
-        <v>346</v>
+        <v>380</v>
       </c>
       <c r="C80" t="s">
-        <v>347</v>
+        <v>381</v>
       </c>
       <c r="D80" t="s">
-        <v>353</v>
-      </c>
-      <c r="E80" t="s">
-        <v>354</v>
+        <v>382</v>
+      </c>
+      <c r="E80">
+        <v>30</v>
       </c>
       <c r="F80" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="H80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>345</v>
+        <v>379</v>
       </c>
       <c r="B81" t="s">
-        <v>348</v>
+        <v>383</v>
       </c>
       <c r="C81" t="s">
-        <v>349</v>
+        <v>384</v>
       </c>
       <c r="D81" t="s">
-        <v>350</v>
-      </c>
-      <c r="E81" t="s">
-        <v>352</v>
+        <v>385</v>
+      </c>
+      <c r="E81">
+        <v>5</v>
       </c>
       <c r="F81" t="s">
-        <v>30</v>
-      </c>
-      <c r="J81" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="H81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>345</v>
+        <v>379</v>
       </c>
       <c r="B82" t="s">
-        <v>355</v>
+        <v>386</v>
       </c>
       <c r="C82" t="s">
-        <v>356</v>
+        <v>387</v>
       </c>
       <c r="D82" t="s">
-        <v>357</v>
-      </c>
-      <c r="E82" t="s">
-        <v>263</v>
+        <v>388</v>
+      </c>
+      <c r="E82">
+        <v>25</v>
       </c>
       <c r="F82" t="s">
-        <v>270</v>
-      </c>
-      <c r="J82" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="H82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>345</v>
+        <v>379</v>
       </c>
       <c r="B83" t="s">
-        <v>358</v>
+        <v>389</v>
       </c>
       <c r="C83" t="s">
-        <v>359</v>
+        <v>66</v>
       </c>
       <c r="D83" t="s">
-        <v>360</v>
+        <v>71</v>
       </c>
       <c r="E83" t="s">
-        <v>361</v>
+        <v>67</v>
       </c>
       <c r="F83" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>345</v>
+        <v>379</v>
       </c>
       <c r="B84" t="s">
-        <v>362</v>
+        <v>390</v>
       </c>
       <c r="C84" t="s">
-        <v>157</v>
+        <v>69</v>
       </c>
       <c r="D84" t="s">
-        <v>363</v>
-      </c>
-      <c r="E84">
-        <v>2010</v>
+        <v>70</v>
+      </c>
+      <c r="E84" t="s">
+        <v>72</v>
       </c>
       <c r="F84" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>345</v>
+        <v>379</v>
       </c>
       <c r="B85" t="s">
-        <v>364</v>
+        <v>391</v>
       </c>
       <c r="C85" t="s">
-        <v>365</v>
+        <v>392</v>
       </c>
       <c r="D85" t="s">
-        <v>366</v>
+        <v>393</v>
       </c>
       <c r="E85" t="s">
-        <v>367</v>
+        <v>394</v>
       </c>
       <c r="F85" t="s">
         <v>13</v>
       </c>
-      <c r="J85" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>345</v>
+        <v>379</v>
       </c>
       <c r="B86" t="s">
-        <v>369</v>
+        <v>395</v>
       </c>
       <c r="C86" t="s">
-        <v>370</v>
+        <v>396</v>
       </c>
       <c r="D86" t="s">
-        <v>371</v>
+        <v>397</v>
       </c>
       <c r="E86" t="s">
-        <v>372</v>
+        <v>398</v>
       </c>
       <c r="F86" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>345</v>
       </c>
       <c r="B87" t="s">
-        <v>373</v>
+        <v>346</v>
       </c>
       <c r="C87" t="s">
-        <v>374</v>
+        <v>347</v>
       </c>
       <c r="D87" t="s">
-        <v>375</v>
-      </c>
-      <c r="E87">
-        <v>0.2</v>
+        <v>353</v>
+      </c>
+      <c r="E87" t="s">
+        <v>354</v>
       </c>
       <c r="F87" t="s">
-        <v>23</v>
-      </c>
-      <c r="H87">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>345</v>
       </c>
       <c r="B88" t="s">
-        <v>376</v>
+        <v>348</v>
       </c>
       <c r="C88" t="s">
-        <v>377</v>
+        <v>349</v>
       </c>
       <c r="D88" t="s">
-        <v>378</v>
-      </c>
-      <c r="E88">
-        <v>14</v>
+        <v>350</v>
+      </c>
+      <c r="E88" t="s">
+        <v>352</v>
       </c>
       <c r="F88" t="s">
-        <v>60</v>
-      </c>
-      <c r="H88">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="J88" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>379</v>
+        <v>345</v>
       </c>
       <c r="B89" t="s">
-        <v>380</v>
+        <v>355</v>
       </c>
       <c r="C89" t="s">
-        <v>381</v>
+        <v>356</v>
       </c>
       <c r="D89" t="s">
-        <v>382</v>
-      </c>
-      <c r="E89">
+        <v>357</v>
+      </c>
+      <c r="E89" t="s">
+        <v>263</v>
+      </c>
+      <c r="F89" t="s">
+        <v>270</v>
+      </c>
+      <c r="J89" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>345</v>
+      </c>
+      <c r="B90" t="s">
+        <v>358</v>
+      </c>
+      <c r="C90" t="s">
+        <v>359</v>
+      </c>
+      <c r="D90" t="s">
+        <v>360</v>
+      </c>
+      <c r="E90" t="s">
+        <v>361</v>
+      </c>
+      <c r="F90" t="s">
         <v>30</v>
       </c>
-      <c r="F89" t="s">
-        <v>60</v>
-      </c>
-      <c r="H89">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>379</v>
-      </c>
-      <c r="B90" t="s">
-        <v>383</v>
-      </c>
-      <c r="C90" t="s">
-        <v>384</v>
-      </c>
-      <c r="D90" t="s">
-        <v>385</v>
-      </c>
-      <c r="E90">
-        <v>5</v>
-      </c>
-      <c r="F90" t="s">
-        <v>60</v>
-      </c>
-      <c r="H90">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>379</v>
+        <v>345</v>
       </c>
       <c r="B91" t="s">
-        <v>386</v>
+        <v>362</v>
       </c>
       <c r="C91" t="s">
-        <v>387</v>
+        <v>157</v>
       </c>
       <c r="D91" t="s">
-        <v>388</v>
+        <v>363</v>
       </c>
       <c r="E91">
-        <v>25</v>
+        <v>2010</v>
       </c>
       <c r="F91" t="s">
-        <v>60</v>
-      </c>
-      <c r="H91">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>379</v>
+        <v>345</v>
       </c>
       <c r="B92" t="s">
-        <v>389</v>
+        <v>364</v>
       </c>
       <c r="C92" t="s">
-        <v>66</v>
+        <v>365</v>
       </c>
       <c r="D92" t="s">
-        <v>71</v>
+        <v>366</v>
       </c>
       <c r="E92" t="s">
-        <v>67</v>
+        <v>367</v>
       </c>
       <c r="F92" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J92" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>379</v>
+        <v>345</v>
       </c>
       <c r="B93" t="s">
-        <v>390</v>
+        <v>369</v>
       </c>
       <c r="C93" t="s">
-        <v>69</v>
+        <v>370</v>
       </c>
       <c r="D93" t="s">
-        <v>70</v>
+        <v>371</v>
       </c>
       <c r="E93" t="s">
-        <v>72</v>
+        <v>372</v>
       </c>
       <c r="F93" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>379</v>
+        <v>345</v>
       </c>
       <c r="B94" t="s">
-        <v>391</v>
+        <v>373</v>
       </c>
       <c r="C94" t="s">
-        <v>392</v>
+        <v>374</v>
       </c>
       <c r="D94" t="s">
-        <v>393</v>
-      </c>
-      <c r="E94" t="s">
-        <v>394</v>
+        <v>375</v>
+      </c>
+      <c r="E94">
+        <v>0.2</v>
       </c>
       <c r="F94" t="s">
-        <v>13</v>
+        <v>23</v>
+      </c>
+      <c r="H94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>345</v>
+      </c>
+      <c r="B95" t="s">
+        <v>376</v>
+      </c>
+      <c r="C95" t="s">
+        <v>377</v>
+      </c>
+      <c r="D95" t="s">
+        <v>378</v>
+      </c>
+      <c r="E95">
+        <v>14</v>
+      </c>
+      <c r="F95" t="s">
+        <v>60</v>
+      </c>
+      <c r="H95">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:T95">
+    <sortCondition ref="A2:A95"/>
+  </sortState>
   <phoneticPr fontId="5" type="noConversion"/>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E32" xr:uid="{914447CD-A1B5-41A0-8105-E69119D5EE3F}">
@@ -3796,12 +3827,12 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="Q15" r:id="rId1" xr:uid="{17C75F52-F5E9-4D49-A18B-8F8976E95C9D}"/>
-    <hyperlink ref="S13" r:id="rId2" xr:uid="{14DC2D8D-2B37-45D3-8BE8-9D92752EC5E1}"/>
-    <hyperlink ref="T12" r:id="rId3" xr:uid="{3832506C-FCCC-4240-AF14-5BFA4AAE2375}"/>
-    <hyperlink ref="T28" r:id="rId4" xr:uid="{A69A80FE-5ACA-4CCB-B5EC-40CF44BD579F}"/>
-    <hyperlink ref="T4" r:id="rId5" xr:uid="{DE9FF68F-0F7A-4E32-9B09-E45F70208747}"/>
-    <hyperlink ref="Q16" r:id="rId6" xr:uid="{AEF445DF-CDFE-4606-8857-0290E102EE35}"/>
+    <hyperlink ref="Q42" r:id="rId1" xr:uid="{17C75F52-F5E9-4D49-A18B-8F8976E95C9D}"/>
+    <hyperlink ref="S40" r:id="rId2" xr:uid="{14DC2D8D-2B37-45D3-8BE8-9D92752EC5E1}"/>
+    <hyperlink ref="T39" r:id="rId3" xr:uid="{3832506C-FCCC-4240-AF14-5BFA4AAE2375}"/>
+    <hyperlink ref="T55" r:id="rId4" xr:uid="{A69A80FE-5ACA-4CCB-B5EC-40CF44BD579F}"/>
+    <hyperlink ref="T24" r:id="rId5" xr:uid="{DE9FF68F-0F7A-4E32-9B09-E45F70208747}"/>
+    <hyperlink ref="Q43" r:id="rId6" xr:uid="{AEF445DF-CDFE-4606-8857-0290E102EE35}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>

</xml_diff>

<commit_message>
update and format table
</commit_message>
<xml_diff>
--- a/experimental_context_description.xlsx
+++ b/experimental_context_description.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vignevin-my.sharepoint.com/personal/xavier_delpuech_vignevin_com/Documents/AgricultureNumerique/ProjetsEnCours/VITISDATACROP/05_TRAVAIL_EN_COURS/WP1.1 Harmonisation/Expérimentation/vitisdatacrop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xdelpuech\OneDrive - vignevin.com\AgricultureNumerique\ProjetsEnCours\VITISDATACROP\05_TRAVAIL_EN_COURS\WP1.1 Harmonisation\Expérimentation\vitisdatacrop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="185" documentId="13_ncr:1_{32B7449F-90EF-4F9B-8AB1-EA4CC5B47857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02FF6B61-D1A8-46AF-9D18-190C1D721350}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{424BCA56-7127-41AC-91C0-F8F969100370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1AE09EEA-C0A3-42DC-AFC7-BA79A75A8C50}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="473">
   <si>
     <t>experimentation</t>
   </si>
@@ -1395,6 +1395,78 @@
   </si>
   <si>
     <t>VAUVERT000BN59</t>
+  </si>
+  <si>
+    <t>3.5</t>
+  </si>
+  <si>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>3500</t>
+  </si>
+  <si>
+    <t>1.5</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>6.5</t>
+  </si>
+  <si>
+    <t>120</t>
+  </si>
+  <si>
+    <t>43.6930</t>
+  </si>
+  <si>
+    <t>4.2784</t>
+  </si>
+  <si>
+    <t>30341</t>
+  </si>
+  <si>
+    <t>1998</t>
+  </si>
+  <si>
+    <t>2.5</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>93</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>215</t>
+  </si>
+  <si>
+    <t>2010</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>0.2</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
   </si>
 </sst>
 </file>
@@ -1472,7 +1544,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -1480,6 +1552,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -1496,10 +1569,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1799,14 +1868,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB13ADFC-DCBE-45B8-93DC-72D8CCE37DD2}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:U105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="38" topLeftCell="G42" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="A39" sqref="A39"/>
-      <selection pane="bottomRight" activeCell="R77" sqref="R77"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="E104" sqref="E104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1883,7 +1948,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="2" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>277</v>
       </c>
@@ -1903,7 +1968,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>277</v>
       </c>
@@ -1923,7 +1988,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>198</v>
       </c>
@@ -1943,7 +2008,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>198</v>
       </c>
@@ -1963,7 +2028,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>198</v>
       </c>
@@ -1986,7 +2051,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="7" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>198</v>
       </c>
@@ -2009,7 +2074,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="8" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>198</v>
       </c>
@@ -2022,14 +2087,14 @@
       <c r="D8" t="s">
         <v>210</v>
       </c>
-      <c r="E8">
-        <v>3</v>
+      <c r="E8" s="7" t="s">
+        <v>463</v>
       </c>
       <c r="F8" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>198</v>
       </c>
@@ -2042,14 +2107,14 @@
       <c r="D9" t="s">
         <v>211</v>
       </c>
-      <c r="E9">
-        <v>215</v>
+      <c r="E9" s="7" t="s">
+        <v>464</v>
       </c>
       <c r="F9" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>198</v>
       </c>
@@ -2069,7 +2134,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>198</v>
       </c>
@@ -2089,7 +2154,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>198</v>
       </c>
@@ -2109,7 +2174,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>198</v>
       </c>
@@ -2132,7 +2197,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="14" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>198</v>
       </c>
@@ -2155,7 +2220,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="15" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>198</v>
       </c>
@@ -2178,7 +2243,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="16" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>198</v>
       </c>
@@ -2201,7 +2266,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="17" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>198</v>
       </c>
@@ -2224,7 +2289,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="18" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>198</v>
       </c>
@@ -2247,7 +2312,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="19" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>198</v>
       </c>
@@ -2270,7 +2335,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="20" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>198</v>
       </c>
@@ -2293,7 +2358,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="21" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>198</v>
       </c>
@@ -2316,7 +2381,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="22" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>198</v>
       </c>
@@ -2339,7 +2404,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="23" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -2365,7 +2430,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="24" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -2397,7 +2462,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="25" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -2426,7 +2491,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="26" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -2449,7 +2514,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>0</v>
       </c>
@@ -2472,7 +2537,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="28" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>0</v>
       </c>
@@ -2498,7 +2563,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="29" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>0</v>
       </c>
@@ -2521,7 +2586,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>0</v>
       </c>
@@ -2544,7 +2609,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="31" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>0</v>
       </c>
@@ -2567,7 +2632,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="32" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>152</v>
       </c>
@@ -2580,8 +2645,8 @@
       <c r="D32" t="s">
         <v>159</v>
       </c>
-      <c r="E32">
-        <v>2010</v>
+      <c r="E32" s="7" t="s">
+        <v>465</v>
       </c>
       <c r="F32" t="s">
         <v>12</v>
@@ -2590,7 +2655,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="33" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>152</v>
       </c>
@@ -2603,8 +2668,8 @@
       <c r="D33" t="s">
         <v>160</v>
       </c>
-      <c r="E33">
-        <v>50</v>
+      <c r="E33" s="7" t="s">
+        <v>466</v>
       </c>
       <c r="F33" t="s">
         <v>22</v>
@@ -2613,7 +2678,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="34" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>152</v>
       </c>
@@ -2626,14 +2691,14 @@
       <c r="D34" t="s">
         <v>161</v>
       </c>
-      <c r="E34">
-        <v>30</v>
+      <c r="E34" s="7" t="s">
+        <v>467</v>
       </c>
       <c r="F34" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>152</v>
       </c>
@@ -2656,7 +2721,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="36" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>152</v>
       </c>
@@ -2676,7 +2741,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>152</v>
       </c>
@@ -2699,7 +2764,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="38" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>152</v>
       </c>
@@ -2732,8 +2797,8 @@
       <c r="D39" t="s">
         <v>26</v>
       </c>
-      <c r="E39">
-        <v>43.692996999999998</v>
+      <c r="E39" s="7" t="s">
+        <v>456</v>
       </c>
       <c r="F39" t="s">
         <v>22</v>
@@ -2770,8 +2835,8 @@
       <c r="D40" t="s">
         <v>27</v>
       </c>
-      <c r="E40">
-        <v>4.2784149999999999</v>
+      <c r="E40" s="7" t="s">
+        <v>457</v>
       </c>
       <c r="F40" t="s">
         <v>22</v>
@@ -2886,8 +2951,8 @@
       <c r="D44" t="s">
         <v>262</v>
       </c>
-      <c r="E44">
-        <v>30341</v>
+      <c r="E44" s="7" t="s">
+        <v>458</v>
       </c>
       <c r="F44" t="s">
         <v>12</v>
@@ -2938,8 +3003,8 @@
       <c r="D46" t="s">
         <v>56</v>
       </c>
-      <c r="E46">
-        <v>1998</v>
+      <c r="E46" s="7" t="s">
+        <v>459</v>
       </c>
       <c r="F46" t="s">
         <v>12</v>
@@ -3027,8 +3092,8 @@
       <c r="D50" t="s">
         <v>71</v>
       </c>
-      <c r="E50">
-        <v>2.5</v>
+      <c r="E50" s="7" t="s">
+        <v>460</v>
       </c>
       <c r="F50" t="s">
         <v>22</v>
@@ -3053,8 +3118,8 @@
       <c r="D51" t="s">
         <v>72</v>
       </c>
-      <c r="E51">
-        <v>1.1000000000000001</v>
+      <c r="E51" s="7" t="s">
+        <v>461</v>
       </c>
       <c r="F51" t="s">
         <v>22</v>
@@ -3157,8 +3222,8 @@
       <c r="D55" t="s">
         <v>73</v>
       </c>
-      <c r="E55">
-        <v>93</v>
+      <c r="E55" s="7" t="s">
+        <v>462</v>
       </c>
       <c r="F55" t="s">
         <v>22</v>
@@ -3316,8 +3381,8 @@
       <c r="D61" t="s">
         <v>115</v>
       </c>
-      <c r="E61">
-        <v>3.5</v>
+      <c r="E61" s="7" t="s">
+        <v>449</v>
       </c>
       <c r="F61" t="s">
         <v>22</v>
@@ -3339,8 +3404,8 @@
       <c r="D62" t="s">
         <v>321</v>
       </c>
-      <c r="E62">
-        <v>0.5</v>
+      <c r="E62" s="7" t="s">
+        <v>450</v>
       </c>
       <c r="F62" t="s">
         <v>22</v>
@@ -3365,8 +3430,8 @@
       <c r="D63" t="s">
         <v>324</v>
       </c>
-      <c r="E63">
-        <v>3500</v>
+      <c r="E63" s="7" t="s">
+        <v>451</v>
       </c>
       <c r="F63" t="s">
         <v>22</v>
@@ -3424,7 +3489,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="66" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>287</v>
       </c>
@@ -3447,7 +3512,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="67" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>287</v>
       </c>
@@ -3467,7 +3532,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="68" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>287</v>
       </c>
@@ -3493,7 +3558,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="69" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>287</v>
       </c>
@@ -3519,7 +3584,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="70" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>287</v>
       </c>
@@ -3539,7 +3604,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="71" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>287</v>
       </c>
@@ -3562,7 +3627,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="72" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>287</v>
       </c>
@@ -3585,7 +3650,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="73" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>287</v>
       </c>
@@ -3605,7 +3670,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="74" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>287</v>
       </c>
@@ -3661,8 +3726,8 @@
       <c r="D76" t="s">
         <v>329</v>
       </c>
-      <c r="E76">
-        <v>1.5</v>
+      <c r="E76" s="7" t="s">
+        <v>452</v>
       </c>
       <c r="F76" t="s">
         <v>22</v>
@@ -3739,8 +3804,8 @@
       <c r="D79" t="s">
         <v>183</v>
       </c>
-      <c r="E79">
-        <v>2</v>
+      <c r="E79" s="7" t="s">
+        <v>453</v>
       </c>
       <c r="F79" t="s">
         <v>22</v>
@@ -3759,8 +3824,8 @@
       <c r="D80" t="s">
         <v>184</v>
       </c>
-      <c r="E80">
-        <v>6.5</v>
+      <c r="E80" s="7" t="s">
+        <v>454</v>
       </c>
       <c r="F80" t="s">
         <v>22</v>
@@ -3779,8 +3844,8 @@
       <c r="D81" t="s">
         <v>409</v>
       </c>
-      <c r="E81">
-        <v>120</v>
+      <c r="E81" s="7" t="s">
+        <v>455</v>
       </c>
       <c r="F81" t="s">
         <v>22</v>
@@ -3818,7 +3883,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="83" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>375</v>
       </c>
@@ -3841,7 +3906,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="84" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>375</v>
       </c>
@@ -3854,8 +3919,8 @@
       <c r="D84" t="s">
         <v>378</v>
       </c>
-      <c r="E84">
-        <v>30</v>
+      <c r="E84" s="7" t="s">
+        <v>467</v>
       </c>
       <c r="F84" t="s">
         <v>57</v>
@@ -3867,7 +3932,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="85" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>375</v>
       </c>
@@ -3880,8 +3945,8 @@
       <c r="D85" t="s">
         <v>381</v>
       </c>
-      <c r="E85">
-        <v>5</v>
+      <c r="E85" s="7" t="s">
+        <v>468</v>
       </c>
       <c r="F85" t="s">
         <v>57</v>
@@ -3893,7 +3958,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="86" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>375</v>
       </c>
@@ -3906,8 +3971,8 @@
       <c r="D86" t="s">
         <v>384</v>
       </c>
-      <c r="E86">
-        <v>25</v>
+      <c r="E86" s="7" t="s">
+        <v>469</v>
       </c>
       <c r="F86" t="s">
         <v>57</v>
@@ -3919,7 +3984,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="87" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>375</v>
       </c>
@@ -3942,7 +4007,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="88" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>375</v>
       </c>
@@ -3965,7 +4030,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="89" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>375</v>
       </c>
@@ -3985,7 +4050,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="90" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>375</v>
       </c>
@@ -4005,7 +4070,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="91" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>341</v>
       </c>
@@ -4025,7 +4090,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="92" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>341</v>
       </c>
@@ -4048,7 +4113,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="93" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>341</v>
       </c>
@@ -4071,7 +4136,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="94" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>341</v>
       </c>
@@ -4091,7 +4156,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="95" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>341</v>
       </c>
@@ -4104,14 +4169,14 @@
       <c r="D95" t="s">
         <v>359</v>
       </c>
-      <c r="E95">
-        <v>2010</v>
+      <c r="E95" s="7" t="s">
+        <v>465</v>
       </c>
       <c r="F95" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="96" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>341</v>
       </c>
@@ -4134,7 +4199,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="97" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>341</v>
       </c>
@@ -4154,7 +4219,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="98" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>341</v>
       </c>
@@ -4167,8 +4232,8 @@
       <c r="D98" t="s">
         <v>371</v>
       </c>
-      <c r="E98">
-        <v>0.2</v>
+      <c r="E98" s="7" t="s">
+        <v>470</v>
       </c>
       <c r="F98" t="s">
         <v>22</v>
@@ -4177,7 +4242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>341</v>
       </c>
@@ -4190,8 +4255,8 @@
       <c r="D99" t="s">
         <v>374</v>
       </c>
-      <c r="E99">
-        <v>14</v>
+      <c r="E99" s="7" t="s">
+        <v>471</v>
       </c>
       <c r="F99" t="s">
         <v>57</v>
@@ -4200,7 +4265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>416</v>
       </c>
@@ -4223,7 +4288,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="101" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>416</v>
       </c>
@@ -4246,7 +4311,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="102" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>416</v>
       </c>
@@ -4269,7 +4334,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="103" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>416</v>
       </c>
@@ -4282,8 +4347,8 @@
       <c r="D103" t="s">
         <v>431</v>
       </c>
-      <c r="E103">
-        <v>15</v>
+      <c r="E103" s="7" t="s">
+        <v>472</v>
       </c>
       <c r="F103" t="s">
         <v>22</v>
@@ -4295,7 +4360,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="104" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>416</v>
       </c>
@@ -4318,7 +4383,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="105" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>416</v>
       </c>
@@ -4339,26 +4404,11 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:T105" xr:uid="{FB13ADFC-DCBE-45B8-93DC-72D8CCE37DD2}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="plot"/>
-        <filter val="soil"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:T105" xr:uid="{FB13ADFC-DCBE-45B8-93DC-72D8CCE37DD2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:T99">
     <sortCondition ref="A2:A99"/>
   </sortState>
   <phoneticPr fontId="5" type="noConversion"/>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E33" xr:uid="{914447CD-A1B5-41A0-8105-E69119D5EE3F}">
-      <formula1>"AOP,IGP,Vins sans IG,Raisin de table"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E32" xr:uid="{97D92A34-09A2-489E-91AE-3F0FC063A126}">
-      <formula1>"Raisonnée ou conventionnelle,Agriculture Biologique,Biodynamie"</formula1>
-    </dataValidation>
-  </dataValidations>
   <hyperlinks>
     <hyperlink ref="Q43" r:id="rId1" xr:uid="{17C75F52-F5E9-4D49-A18B-8F8976E95C9D}"/>
     <hyperlink ref="S41" r:id="rId2" xr:uid="{14DC2D8D-2B37-45D3-8BE8-9D92752EC5E1}"/>

</xml_diff>

<commit_message>
suppression déclaration du suivi expé
</commit_message>
<xml_diff>
--- a/experimental_context_description.xlsx
+++ b/experimental_context_description.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vignevin-my.sharepoint.com/personal/xavier_delpuech_vignevin_com/Documents/AgricultureNumerique/ProjetsEnCours/VITISDATACROP/05_TRAVAIL_EN_COURS/WP1.1 Harmonisation/Expérimentation/vitisdatacrop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="188" documentId="13_ncr:1_{408E4E9B-A7F7-4609-9E19-471F8CD70632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ADACD91A-CDAC-40E6-A054-58A83A2E41D2}"/>
+  <xr:revisionPtr revIDLastSave="192" documentId="13_ncr:1_{408E4E9B-A7F7-4609-9E19-471F8CD70632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{40E733AB-333D-49C3-867F-61D104CA3F42}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1AE09EEA-C0A3-42DC-AFC7-BA79A75A8C50}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="512">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="476">
   <si>
     <t>experimentation</t>
   </si>
@@ -714,79 +714,7 @@
     <t>http://purl.obolibrary.org/obo/CO_715_0000253</t>
   </si>
   <si>
-    <t>Capteurs</t>
-  </si>
-  <si>
-    <t>Descriptifs des capteurs équipant la parcelle le cas échéant</t>
-  </si>
-  <si>
-    <t>sonde d'humidité des sols de typa capacitive</t>
-  </si>
-  <si>
-    <t>Performances agronomiques</t>
-  </si>
-  <si>
-    <t>Statut hydrique de la vigne</t>
-  </si>
-  <si>
-    <t>Statut minéral de la vigne</t>
-  </si>
-  <si>
-    <t>Analyses de sols</t>
-  </si>
-  <si>
-    <t>Suivi maladies</t>
-  </si>
-  <si>
-    <t>Analyse maturité</t>
-  </si>
-  <si>
-    <t>Vinification</t>
-  </si>
-  <si>
-    <t>Analyses sensorielles</t>
-  </si>
-  <si>
-    <t>Suivi couverts végétaux</t>
-  </si>
-  <si>
-    <t>Données météo</t>
-  </si>
-  <si>
-    <t>Mesures de Performances agronomiques réalisées</t>
-  </si>
-  <si>
-    <t>Mesures de Statut hydrique de la vigne réalisées</t>
-  </si>
-  <si>
-    <t>Mesures de Statut minéral de la vigne réalisées</t>
-  </si>
-  <si>
-    <t>Mesures de Analyses de sols réalisées</t>
-  </si>
-  <si>
-    <t>Mesures de Suivi maladies réalisées</t>
-  </si>
-  <si>
-    <t>Mesures de Analyse maturité réalisées</t>
-  </si>
-  <si>
-    <t>Mesures de Vinification réalisées</t>
-  </si>
-  <si>
-    <t>Mesures de Analyses sensorielles réalisées</t>
-  </si>
-  <si>
-    <t>Mesures de Suivi couverts végétaux réalisées</t>
-  </si>
-  <si>
-    <t>Mesures de Données météo réalisées</t>
-  </si>
-  <si>
     <t>oui</t>
-  </si>
-  <si>
-    <t>non</t>
   </si>
   <si>
     <t>oui,non</t>
@@ -1416,42 +1344,6 @@
   </si>
   <si>
     <t>Code du traitement expérimental appliqué ou en lien avec le vin</t>
-  </si>
-  <si>
-    <t>monitoring</t>
-  </si>
-  <si>
-    <t>monitoring_device</t>
-  </si>
-  <si>
-    <t>monitoring_obs_agro</t>
-  </si>
-  <si>
-    <t>monitoring_obs_hyd</t>
-  </si>
-  <si>
-    <t>monitoring_obs_min</t>
-  </si>
-  <si>
-    <t>monitoring_obs_soil</t>
-  </si>
-  <si>
-    <t>monitoring_obs_dis</t>
-  </si>
-  <si>
-    <t>monitoring_obs_mat</t>
-  </si>
-  <si>
-    <t>monitoring_obs_vin</t>
-  </si>
-  <si>
-    <t>monitoring_obs_sen</t>
-  </si>
-  <si>
-    <t>monitoring_obs_cc</t>
-  </si>
-  <si>
-    <t>monitoring_obs_mto</t>
   </si>
   <si>
     <t>priority</t>
@@ -1700,10 +1592,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2003,11 +1891,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB13ADFC-DCBE-45B8-93DC-72D8CCE37DD2}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:V112"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D90" sqref="D90"/>
+      <selection activeCell="A15" sqref="A15:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="67.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2056,7 +1943,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>469</v>
+        <v>433</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>5</v>
@@ -2092,7 +1979,7 @@
         <v>214</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>475</v>
+        <v>439</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>215</v>
@@ -2101,50 +1988,50 @@
         <v>217</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" ht="135.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" ht="135.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>255</v>
+        <v>231</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>257</v>
+        <v>233</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>258</v>
+        <v>234</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>260</v>
+        <v>236</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>256</v>
+        <v>232</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>259</v>
+        <v>235</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>261</v>
+        <v>237</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>262</v>
+        <v>238</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>192</v>
       </c>
@@ -2164,88 +2051,88 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>486</v>
+        <v>450</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>494</v>
+        <v>458</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>488</v>
+        <v>452</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>480</v>
+        <v>444</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>481</v>
+        <v>445</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>484</v>
+        <v>448</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>486</v>
+        <v>450</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>362</v>
+        <v>338</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>363</v>
+        <v>339</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>364</v>
+        <v>340</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>365</v>
+        <v>341</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>26</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>483</v>
+        <v>447</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>486</v>
+        <v>450</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>478</v>
+        <v>442</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>490</v>
+        <v>454</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>492</v>
+        <v>456</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>491</v>
+        <v>455</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>26</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>482</v>
+        <v>446</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>192</v>
       </c>
@@ -2268,47 +2155,47 @@
         <v>207</v>
       </c>
     </row>
-    <row r="9" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>192</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>485</v>
+        <v>449</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>360</v>
+        <v>336</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>495</v>
+        <v>459</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>496</v>
+        <v>460</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>192</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>497</v>
+        <v>461</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>498</v>
+        <v>462</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>499</v>
+        <v>463</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>502</v>
+        <v>466</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>192</v>
       </c>
@@ -2316,19 +2203,19 @@
         <v>210</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>500</v>
+        <v>464</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>501</v>
+        <v>465</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>425</v>
+        <v>401</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>192</v>
       </c>
@@ -2342,13 +2229,13 @@
         <v>201</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>426</v>
+        <v>402</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:22" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>192</v>
       </c>
@@ -2368,7 +2255,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>192</v>
       </c>
@@ -2388,257 +2275,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:22" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>457</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>457</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>459</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>457</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>460</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>457</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>461</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>457</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>462</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>457</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>463</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>457</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>464</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>457</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>465</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>457</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>466</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>457</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>467</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>457</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>468</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>0</v>
       </c>
@@ -2649,7 +2286,7 @@
         <v>135</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>368</v>
+        <v>344</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>131</v>
@@ -2661,10 +2298,10 @@
         <v>1</v>
       </c>
       <c r="R26" s="2" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>0</v>
       </c>
@@ -2690,13 +2327,13 @@
         <v>18</v>
       </c>
       <c r="R27" s="2" t="s">
-        <v>435</v>
+        <v>411</v>
       </c>
       <c r="U27" s="6" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>0</v>
       </c>
@@ -2722,13 +2359,13 @@
         <v>18</v>
       </c>
       <c r="R28" s="2" t="s">
-        <v>435</v>
+        <v>411</v>
       </c>
       <c r="U28" s="7" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="29" spans="1:21" ht="225" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" ht="225" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>0</v>
       </c>
@@ -2751,10 +2388,10 @@
         <v>1</v>
       </c>
       <c r="R29" s="2" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21" ht="165" hidden="1" x14ac:dyDescent="0.25">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" ht="165" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>0</v>
       </c>
@@ -2774,10 +2411,10 @@
         <v>12</v>
       </c>
       <c r="R30" s="2" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>0</v>
       </c>
@@ -2800,10 +2437,10 @@
         <v>1</v>
       </c>
       <c r="R31" s="2" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>0</v>
       </c>
@@ -2826,10 +2463,10 @@
         <v>2</v>
       </c>
       <c r="R32" s="2" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="33" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>0</v>
       </c>
@@ -2849,10 +2486,10 @@
         <v>12</v>
       </c>
       <c r="R33" s="2" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="34" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>0</v>
       </c>
@@ -2875,10 +2512,10 @@
         <v>114</v>
       </c>
       <c r="R34" s="2" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="35" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>147</v>
       </c>
@@ -2892,16 +2529,16 @@
         <v>154</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>427</v>
+        <v>403</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>12</v>
       </c>
       <c r="R35" s="2" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="36" spans="1:21" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>147</v>
       </c>
@@ -2915,16 +2552,16 @@
         <v>155</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>428</v>
+        <v>404</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>20</v>
       </c>
       <c r="R36" s="2" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="37" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>147</v>
       </c>
@@ -2938,13 +2575,13 @@
         <v>156</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>429</v>
+        <v>405</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>147</v>
       </c>
@@ -2967,7 +2604,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="39" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>147</v>
       </c>
@@ -2987,33 +2624,33 @@
         <v>12</v>
       </c>
       <c r="R39" s="2" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="40" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>147</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>310</v>
+        <v>286</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>311</v>
+        <v>287</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>312</v>
+        <v>288</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>313</v>
+        <v>289</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>26</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="41" spans="1:21" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>147</v>
       </c>
@@ -3024,7 +2661,7 @@
         <v>153</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>471</v>
+        <v>435</v>
       </c>
       <c r="E41" s="2">
         <v>0</v>
@@ -3033,7 +2670,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>19</v>
       </c>
@@ -3047,7 +2684,7 @@
         <v>23</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>418</v>
+        <v>394</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>20</v>
@@ -3065,13 +2702,13 @@
         <v>43.692996999999998</v>
       </c>
       <c r="R42" s="2" t="s">
-        <v>442</v>
+        <v>418</v>
       </c>
       <c r="U42" s="8" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="43" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>19</v>
       </c>
@@ -3085,7 +2722,7 @@
         <v>24</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>419</v>
+        <v>395</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>20</v>
@@ -3103,13 +2740,13 @@
         <v>4.2784149999999999</v>
       </c>
       <c r="R43" s="2" t="s">
-        <v>442</v>
+        <v>418</v>
       </c>
       <c r="U43" s="7" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="44" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>19</v>
       </c>
@@ -3120,7 +2757,7 @@
         <v>38</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>369</v>
+        <v>345</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>29</v>
@@ -3132,13 +2769,13 @@
         <v>1</v>
       </c>
       <c r="R44" s="2" t="s">
-        <v>437</v>
+        <v>413</v>
       </c>
       <c r="T44" s="7" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="45" spans="1:21" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>19</v>
       </c>
@@ -3149,7 +2786,7 @@
         <v>37</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>406</v>
+        <v>382</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>39</v>
@@ -3158,10 +2795,10 @@
         <v>12</v>
       </c>
       <c r="R45" s="2" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="46" spans="1:21" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>19</v>
       </c>
@@ -3184,39 +2821,39 @@
         <v>44</v>
       </c>
       <c r="R46" s="2" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="47" spans="1:21" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>250</v>
+        <v>226</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>249</v>
+        <v>225</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>420</v>
+        <v>396</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>12</v>
       </c>
       <c r="L47" s="2" t="s">
-        <v>252</v>
+        <v>228</v>
       </c>
       <c r="Q47" s="7" t="s">
         <v>44</v>
       </c>
       <c r="R47" s="2" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="48" spans="1:21" ht="60" hidden="1" x14ac:dyDescent="0.25">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>19</v>
       </c>
@@ -3239,7 +2876,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="49" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>19</v>
       </c>
@@ -3253,7 +2890,7 @@
         <v>53</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>421</v>
+        <v>397</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>12</v>
@@ -3262,10 +2899,10 @@
         <v>1</v>
       </c>
       <c r="R49" s="2" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="50" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>19</v>
       </c>
@@ -3285,7 +2922,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="51" spans="1:21" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>19</v>
       </c>
@@ -3308,10 +2945,10 @@
         <v>1</v>
       </c>
       <c r="R51" s="2" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="52" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>19</v>
       </c>
@@ -3334,10 +2971,10 @@
         <v>1</v>
       </c>
       <c r="R52" s="2" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="53" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>19</v>
       </c>
@@ -3351,7 +2988,7 @@
         <v>68</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>422</v>
+        <v>398</v>
       </c>
       <c r="F53" s="2" t="s">
         <v>20</v>
@@ -3360,10 +2997,10 @@
         <v>0</v>
       </c>
       <c r="R53" s="2" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="54" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>19</v>
       </c>
@@ -3377,7 +3014,7 @@
         <v>69</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>423</v>
+        <v>399</v>
       </c>
       <c r="F54" s="2" t="s">
         <v>20</v>
@@ -3386,10 +3023,10 @@
         <v>0</v>
       </c>
       <c r="R54" s="2" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="55" spans="1:21" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>19</v>
       </c>
@@ -3409,13 +3046,13 @@
         <v>26</v>
       </c>
       <c r="J55" s="2" t="s">
-        <v>304</v>
+        <v>280</v>
       </c>
       <c r="R55" s="2" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="56" spans="1:21" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>19</v>
       </c>
@@ -3435,13 +3072,13 @@
         <v>26</v>
       </c>
       <c r="J56" s="2" t="s">
-        <v>305</v>
+        <v>281</v>
       </c>
       <c r="R56" s="2" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="57" spans="1:21" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>19</v>
       </c>
@@ -3464,10 +3101,10 @@
         <v>27</v>
       </c>
       <c r="R57" s="2" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="58" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>19</v>
       </c>
@@ -3481,7 +3118,7 @@
         <v>70</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>424</v>
+        <v>400</v>
       </c>
       <c r="F58" s="2" t="s">
         <v>20</v>
@@ -3493,7 +3130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:21" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>19</v>
       </c>
@@ -3528,7 +3165,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="60" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>19</v>
       </c>
@@ -3539,7 +3176,7 @@
         <v>78</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>450</v>
+        <v>426</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>97</v>
@@ -3554,10 +3191,10 @@
         <v>106</v>
       </c>
       <c r="R60" s="2" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="61" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>19</v>
       </c>
@@ -3568,7 +3205,7 @@
         <v>79</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>449</v>
+        <v>425</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>97</v>
@@ -3583,24 +3220,24 @@
         <v>107</v>
       </c>
       <c r="R61" s="2" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="62" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>445</v>
+        <v>421</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>446</v>
+        <v>422</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>447</v>
+        <v>423</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>448</v>
+        <v>424</v>
       </c>
       <c r="F62" s="2" t="s">
         <v>12</v>
@@ -3609,10 +3246,10 @@
         <v>2</v>
       </c>
       <c r="R62" s="2" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="63" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>19</v>
       </c>
@@ -3638,10 +3275,10 @@
         <v>108</v>
       </c>
       <c r="R63" s="2" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="64" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>19</v>
       </c>
@@ -3664,13 +3301,13 @@
         <v>2</v>
       </c>
       <c r="J64" s="2" t="s">
-        <v>378</v>
+        <v>354</v>
       </c>
       <c r="R64" s="2" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="65" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>19</v>
       </c>
@@ -3684,7 +3321,7 @@
         <v>110</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>411</v>
+        <v>387</v>
       </c>
       <c r="F65" s="2" t="s">
         <v>20</v>
@@ -3696,21 +3333,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>293</v>
+        <v>269</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>294</v>
+        <v>270</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>295</v>
+        <v>271</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>412</v>
+        <v>388</v>
       </c>
       <c r="F66" s="2" t="s">
         <v>20</v>
@@ -3722,24 +3359,24 @@
         <v>0</v>
       </c>
       <c r="R66" s="2" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="67" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>296</v>
+        <v>272</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>297</v>
+        <v>273</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>298</v>
+        <v>274</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>413</v>
+        <v>389</v>
       </c>
       <c r="F67" s="2" t="s">
         <v>20</v>
@@ -3748,24 +3385,24 @@
         <v>1</v>
       </c>
       <c r="R67" s="2" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="68" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>407</v>
+        <v>383</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>409</v>
+        <v>385</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>408</v>
+        <v>384</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>410</v>
+        <v>386</v>
       </c>
       <c r="F68" s="2" t="s">
         <v>12</v>
@@ -3774,24 +3411,24 @@
         <v>3</v>
       </c>
       <c r="R68" s="2" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="69" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>299</v>
+        <v>275</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>300</v>
+        <v>276</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>300</v>
+        <v>276</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>301</v>
+        <v>277</v>
       </c>
       <c r="F69" s="2" t="s">
         <v>12</v>
@@ -3800,27 +3437,27 @@
         <v>2</v>
       </c>
       <c r="J69" s="2" t="s">
-        <v>302</v>
+        <v>278</v>
       </c>
       <c r="R69" s="2" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="70" spans="1:20" ht="60" hidden="1" x14ac:dyDescent="0.25">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="70" spans="1:20" ht="60" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>263</v>
+        <v>239</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>473</v>
+        <v>437</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>474</v>
+        <v>438</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>474</v>
+        <v>438</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>274</v>
+        <v>250</v>
       </c>
       <c r="F70" s="2" t="s">
         <v>12</v>
@@ -3829,25 +3466,25 @@
         <v>1</v>
       </c>
       <c r="R70" s="2" t="s">
-        <v>472</v>
+        <v>436</v>
       </c>
       <c r="S70" s="2" t="s">
-        <v>476</v>
+        <v>440</v>
       </c>
       <c r="T70" s="7"/>
     </row>
-    <row r="71" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>263</v>
+        <v>239</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>284</v>
+        <v>260</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>267</v>
+        <v>243</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>264</v>
+        <v>240</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>126</v>
@@ -3859,24 +3496,24 @@
         <v>3</v>
       </c>
       <c r="R71" s="2" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="72" spans="1:20" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="72" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>263</v>
+        <v>239</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>286</v>
+        <v>262</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>268</v>
+        <v>244</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>282</v>
+        <v>258</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>275</v>
+        <v>251</v>
       </c>
       <c r="F72" s="2" t="s">
         <v>17</v>
@@ -3888,24 +3525,24 @@
         <v>18</v>
       </c>
       <c r="R72" s="2" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="73" spans="1:20" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B73" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="B73" s="2" t="s">
-        <v>287</v>
-      </c>
       <c r="C73" s="2" t="s">
-        <v>269</v>
+        <v>245</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>283</v>
+        <v>259</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>276</v>
+        <v>252</v>
       </c>
       <c r="F73" s="2" t="s">
         <v>17</v>
@@ -3917,24 +3554,24 @@
         <v>18</v>
       </c>
       <c r="R73" s="2" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="74" spans="1:20" ht="285" hidden="1" x14ac:dyDescent="0.25">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="74" spans="1:20" ht="285" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>263</v>
+        <v>239</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>288</v>
+        <v>264</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>116</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>265</v>
+        <v>241</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>277</v>
+        <v>253</v>
       </c>
       <c r="F74" s="2" t="s">
         <v>12</v>
@@ -3943,24 +3580,24 @@
         <v>2</v>
       </c>
       <c r="R74" s="2" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="75" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="75" spans="1:20" ht="135" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>263</v>
+        <v>239</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>289</v>
+        <v>265</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>117</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>266</v>
+        <v>242</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>278</v>
+        <v>254</v>
       </c>
       <c r="F75" s="2" t="s">
         <v>12</v>
@@ -3969,27 +3606,27 @@
         <v>1</v>
       </c>
       <c r="R75" s="2" t="s">
-        <v>472</v>
+        <v>436</v>
       </c>
       <c r="S75" s="2" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="76" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>263</v>
+        <v>239</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>290</v>
+        <v>266</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>270</v>
+        <v>246</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>292</v>
+        <v>268</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>279</v>
+        <v>255</v>
       </c>
       <c r="F76" s="2" t="s">
         <v>12</v>
@@ -3998,24 +3635,24 @@
         <v>2</v>
       </c>
       <c r="R76" s="2" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="77" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>263</v>
+        <v>239</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>291</v>
+        <v>267</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>271</v>
+        <v>247</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>113</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>280</v>
+        <v>256</v>
       </c>
       <c r="F77" s="2" t="s">
         <v>132</v>
@@ -4024,24 +3661,24 @@
         <v>3</v>
       </c>
       <c r="R77" s="2" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="78" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>263</v>
+        <v>239</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>285</v>
+        <v>261</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>272</v>
+        <v>248</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>273</v>
+        <v>249</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>281</v>
+        <v>257</v>
       </c>
       <c r="F78" s="2" t="s">
         <v>12</v>
@@ -4050,10 +3687,10 @@
         <v>2</v>
       </c>
       <c r="R78" s="2" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="79" spans="1:20" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="79" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>168</v>
       </c>
@@ -4076,10 +3713,10 @@
         <v>1</v>
       </c>
       <c r="R79" s="2" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="80" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>168</v>
       </c>
@@ -4090,10 +3727,10 @@
         <v>170</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>303</v>
+        <v>279</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>414</v>
+        <v>390</v>
       </c>
       <c r="F80" s="2" t="s">
         <v>20</v>
@@ -4102,10 +3739,10 @@
         <v>2</v>
       </c>
       <c r="R80" s="2" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="81" spans="1:22" ht="60" hidden="1" x14ac:dyDescent="0.25">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="81" spans="1:22" ht="60" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>168</v>
       </c>
@@ -4134,10 +3771,10 @@
         <v>186</v>
       </c>
       <c r="R81" s="2" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="82" spans="1:22" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="82" spans="1:22" ht="45" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>168</v>
       </c>
@@ -4166,10 +3803,10 @@
         <v>109</v>
       </c>
       <c r="R82" s="2" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="83" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="83" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>168</v>
       </c>
@@ -4183,7 +3820,7 @@
         <v>177</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>415</v>
+        <v>391</v>
       </c>
       <c r="F83" s="2" t="s">
         <v>20</v>
@@ -4192,7 +3829,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>168</v>
       </c>
@@ -4206,7 +3843,7 @@
         <v>178</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>416</v>
+        <v>392</v>
       </c>
       <c r="F84" s="2" t="s">
         <v>20</v>
@@ -4215,21 +3852,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:22" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>168</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>372</v>
+        <v>348</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>373</v>
+        <v>349</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>470</v>
+        <v>434</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>417</v>
+        <v>393</v>
       </c>
       <c r="F85" s="2" t="s">
         <v>20</v>
@@ -4241,24 +3878,24 @@
         <v>0</v>
       </c>
       <c r="V85" s="2" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="86" spans="1:22" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="86" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>168</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>306</v>
+        <v>282</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>307</v>
+        <v>283</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>307</v>
+        <v>283</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>309</v>
+        <v>285</v>
       </c>
       <c r="F86" s="2" t="s">
         <v>26</v>
@@ -4267,50 +3904,50 @@
         <v>3</v>
       </c>
       <c r="J86" s="2" t="s">
-        <v>308</v>
+        <v>284</v>
       </c>
       <c r="V86" s="2" t="s">
-        <v>376</v>
+        <v>352</v>
       </c>
     </row>
     <row r="87" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>349</v>
+        <v>325</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>370</v>
+        <v>346</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>503</v>
+        <v>467</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>504</v>
+        <v>468</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="F87" s="2" t="s">
         <v>12</v>
       </c>
       <c r="R87" s="2" t="s">
-        <v>439</v>
+        <v>415</v>
       </c>
     </row>
     <row r="88" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>349</v>
+        <v>325</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>350</v>
+        <v>326</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>351</v>
+        <v>327</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>505</v>
+        <v>469</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>429</v>
+        <v>405</v>
       </c>
       <c r="F88" s="2" t="s">
         <v>54</v>
@@ -4319,24 +3956,24 @@
         <v>0</v>
       </c>
       <c r="R88" s="2" t="s">
-        <v>439</v>
+        <v>415</v>
       </c>
     </row>
     <row r="89" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>349</v>
+        <v>325</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>352</v>
+        <v>328</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>506</v>
+        <v>470</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>509</v>
+        <v>473</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>430</v>
+        <v>406</v>
       </c>
       <c r="F89" s="2" t="s">
         <v>54</v>
@@ -4345,24 +3982,24 @@
         <v>0</v>
       </c>
       <c r="R89" s="2" t="s">
-        <v>439</v>
+        <v>415</v>
       </c>
     </row>
     <row r="90" spans="1:22" ht="45" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>349</v>
+        <v>325</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>353</v>
+        <v>329</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>507</v>
+        <v>471</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>508</v>
+        <v>472</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>431</v>
+        <v>407</v>
       </c>
       <c r="F90" s="2" t="s">
         <v>54</v>
@@ -4371,12 +4008,12 @@
         <v>0</v>
       </c>
       <c r="R90" s="2" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="91" spans="1:22" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="91" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="B91" s="2" t="s">
-        <v>354</v>
+        <v>330</v>
       </c>
       <c r="C91" s="2" t="s">
         <v>60</v>
@@ -4394,12 +4031,12 @@
         <v>3</v>
       </c>
       <c r="R91" s="2" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="92" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="92" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B92" s="2" t="s">
-        <v>355</v>
+        <v>331</v>
       </c>
       <c r="C92" s="2" t="s">
         <v>63</v>
@@ -4417,240 +4054,240 @@
         <v>3</v>
       </c>
       <c r="R92" s="2" t="s">
-        <v>439</v>
+        <v>415</v>
       </c>
     </row>
     <row r="93" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>349</v>
+        <v>325</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>356</v>
+        <v>332</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>357</v>
+        <v>333</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>510</v>
+        <v>474</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>358</v>
+        <v>334</v>
       </c>
       <c r="F93" s="2" t="s">
         <v>12</v>
       </c>
       <c r="R93" s="2" t="s">
-        <v>440</v>
+        <v>416</v>
       </c>
     </row>
     <row r="94" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>349</v>
+        <v>325</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>359</v>
+        <v>335</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>360</v>
+        <v>336</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>511</v>
+        <v>475</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>361</v>
+        <v>337</v>
       </c>
       <c r="F94" s="2" t="s">
         <v>12</v>
       </c>
       <c r="R94" s="2" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="95" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="95" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>315</v>
+        <v>291</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>316</v>
+        <v>292</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>317</v>
+        <v>293</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>323</v>
+        <v>299</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>324</v>
+        <v>300</v>
       </c>
       <c r="F95" s="2" t="s">
         <v>26</v>
       </c>
       <c r="R95" s="2" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="96" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="96" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>315</v>
+        <v>291</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>318</v>
+        <v>294</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>319</v>
+        <v>295</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>320</v>
+        <v>296</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>322</v>
+        <v>298</v>
       </c>
       <c r="F96" s="2" t="s">
         <v>26</v>
       </c>
       <c r="J96" s="2" t="s">
-        <v>321</v>
+        <v>297</v>
       </c>
       <c r="R96" s="2" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="97" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>315</v>
+        <v>291</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>326</v>
+        <v>302</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>327</v>
+        <v>303</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>246</v>
+        <v>223</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>253</v>
+        <v>229</v>
       </c>
       <c r="J97" s="2" t="s">
-        <v>248</v>
+        <v>224</v>
       </c>
       <c r="R97" s="2" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="98" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>315</v>
+        <v>291</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>328</v>
+        <v>304</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>329</v>
+        <v>305</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>330</v>
+        <v>306</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>331</v>
+        <v>307</v>
       </c>
       <c r="F98" s="2" t="s">
         <v>26</v>
       </c>
       <c r="R98" s="2" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="99" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>315</v>
+        <v>291</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>332</v>
+        <v>308</v>
       </c>
       <c r="C99" s="2" t="s">
         <v>148</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>333</v>
+        <v>309</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>427</v>
+        <v>403</v>
       </c>
       <c r="F99" s="2" t="s">
         <v>12</v>
       </c>
       <c r="R99" s="2" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="100" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>315</v>
+        <v>291</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>334</v>
+        <v>310</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>335</v>
+        <v>311</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>336</v>
+        <v>312</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>337</v>
+        <v>313</v>
       </c>
       <c r="F100" s="2" t="s">
         <v>26</v>
       </c>
       <c r="J100" s="2" t="s">
-        <v>338</v>
+        <v>314</v>
       </c>
       <c r="R100" s="2" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="101" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="B101" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="B101" s="2" t="s">
-        <v>339</v>
-      </c>
       <c r="C101" s="2" t="s">
-        <v>340</v>
+        <v>316</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>341</v>
+        <v>317</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>342</v>
+        <v>318</v>
       </c>
       <c r="F101" s="2" t="s">
         <v>12</v>
       </c>
       <c r="R101" s="2" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="102" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="102" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>315</v>
+        <v>291</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>343</v>
+        <v>319</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>344</v>
+        <v>320</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>345</v>
+        <v>321</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>432</v>
+        <v>408</v>
       </c>
       <c r="F102" s="2" t="s">
         <v>20</v>
@@ -4659,24 +4296,24 @@
         <v>0</v>
       </c>
       <c r="R102" s="2" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="103" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="103" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>315</v>
+        <v>291</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>346</v>
+        <v>322</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>348</v>
+        <v>324</v>
       </c>
       <c r="E103" s="3" t="s">
-        <v>433</v>
+        <v>409</v>
       </c>
       <c r="F103" s="2" t="s">
         <v>54</v>
@@ -4685,93 +4322,93 @@
         <v>0</v>
       </c>
       <c r="R103" s="2" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="104" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="104" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>379</v>
+        <v>355</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>380</v>
+        <v>356</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>381</v>
+        <v>357</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>382</v>
+        <v>358</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>387</v>
+        <v>363</v>
       </c>
       <c r="F104" s="2" t="s">
         <v>12</v>
       </c>
       <c r="R104" s="2" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="105" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
-        <v>379</v>
+        <v>355</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>383</v>
+        <v>359</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>384</v>
+        <v>360</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>385</v>
+        <v>361</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>386</v>
+        <v>362</v>
       </c>
       <c r="F105" s="2" t="s">
         <v>12</v>
       </c>
       <c r="R105" s="2" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="106" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="106" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>379</v>
+        <v>355</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>388</v>
+        <v>364</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>389</v>
+        <v>365</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>390</v>
+        <v>366</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>391</v>
+        <v>367</v>
       </c>
       <c r="F106" s="2" t="s">
         <v>12</v>
       </c>
       <c r="R106" s="2" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="107" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="107" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>379</v>
+        <v>355</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>392</v>
+        <v>368</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>393</v>
+        <v>369</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>394</v>
+        <v>370</v>
       </c>
       <c r="E107" s="3" t="s">
-        <v>434</v>
+        <v>410</v>
       </c>
       <c r="F107" s="2" t="s">
         <v>20</v>
@@ -4780,126 +4417,120 @@
         <v>0</v>
       </c>
       <c r="R107" s="2" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="108" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="108" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="F108" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L108" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="R108" s="2" t="s">
         <v>379</v>
       </c>
-      <c r="B108" s="2" t="s">
-        <v>397</v>
-      </c>
-      <c r="C108" s="2" t="s">
-        <v>398</v>
-      </c>
-      <c r="D108" s="2" t="s">
-        <v>401</v>
-      </c>
-      <c r="F108" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="L108" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="R108" s="2" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="109" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="109" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>379</v>
+        <v>355</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>399</v>
+        <v>375</v>
       </c>
       <c r="C109" s="2" t="s">
         <v>117</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>400</v>
+        <v>376</v>
       </c>
       <c r="F109" s="2" t="s">
         <v>12</v>
       </c>
       <c r="R109" s="2" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="110" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="110" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>315</v>
+        <v>291</v>
       </c>
       <c r="B110" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="E110" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="F110" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="R110" s="2" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="111" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A111" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="E111" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="F111" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="R111" s="2" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="112" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A112" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="B112" s="2" t="s">
         <v>451</v>
       </c>
-      <c r="C110" s="2" t="s">
-        <v>452</v>
-      </c>
-      <c r="D110" s="2" t="s">
+      <c r="C112" s="2" t="s">
         <v>453</v>
       </c>
-      <c r="E110" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="F110" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="R110" s="2" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="111" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>455</v>
-      </c>
-      <c r="C111" s="2" t="s">
-        <v>360</v>
-      </c>
-      <c r="D111" s="2" t="s">
-        <v>456</v>
-      </c>
-      <c r="E111" s="2" t="s">
-        <v>361</v>
-      </c>
-      <c r="F111" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="R111" s="2" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="112" spans="1:18" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="2" t="s">
-        <v>486</v>
-      </c>
-      <c r="B112" s="2" t="s">
-        <v>487</v>
-      </c>
-      <c r="C112" s="2" t="s">
-        <v>489</v>
-      </c>
       <c r="D112" s="2" t="s">
-        <v>489</v>
+        <v>453</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>493</v>
+        <v>457</v>
       </c>
       <c r="F112" s="2" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:U112" xr:uid="{FB13ADFC-DCBE-45B8-93DC-72D8CCE37DD2}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="subplot"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:U112" xr:uid="{FB13ADFC-DCBE-45B8-93DC-72D8CCE37DD2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U103">
     <sortCondition ref="A2:A103"/>
   </sortState>

</xml_diff>

<commit_message>
move number of repetion from design to treatments description
the number of repetition could vary between treatments
</commit_message>
<xml_diff>
--- a/experimental_context_description.xlsx
+++ b/experimental_context_description.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vignevin-my.sharepoint.com/personal/xavier_delpuech_vignevin_com/Documents/AgricultureNumerique/ProjetsEnCours/VITISDATACROP/05_TRAVAIL_EN_COURS/WP1.1 Harmonisation/Expérimentation/vitisdatacrop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="125" documentId="13_ncr:1_{7E65C6BA-C87A-4619-9764-C45083FA781A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A20FEF2C-B88B-4AA0-88E8-83F23A88CB93}"/>
+  <xr:revisionPtr revIDLastSave="141" documentId="13_ncr:1_{7E65C6BA-C87A-4619-9764-C45083FA781A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B97445D4-E882-4FDB-8D0C-8F842C9D3917}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1AE09EEA-C0A3-42DC-AFC7-BA79A75A8C50}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1AE09EEA-C0A3-42DC-AFC7-BA79A75A8C50}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -1483,9 +1483,6 @@
     <t>false</t>
   </si>
   <si>
-    <t>Nombre de répétitions par traitement expérimental (combinaison de facteurs appliqués)</t>
-  </si>
-  <si>
     <t>Nom de la variété (et clone si connu) du porte-greffe. Utiliser la liste disposnible sur https://vitioeno.mistea.inrae.fr/resource/app/germplasm</t>
   </si>
   <si>
@@ -1714,9 +1711,6 @@
     <t>treatment_name</t>
   </si>
   <si>
-    <t>Nom ou code du traitement</t>
-  </si>
-  <si>
     <t>treatment</t>
   </si>
   <si>
@@ -1726,12 +1720,6 @@
     <t>Commentaires</t>
   </si>
   <si>
-    <t>Commentaires sur le traitement</t>
-  </si>
-  <si>
-    <t>Liste des niveaux de facteurs du traitement (séparés par ";")</t>
-  </si>
-  <si>
     <t>unit</t>
   </si>
   <si>
@@ -1853,6 +1841,18 @@
   </si>
   <si>
     <t>Nom de la parcelle expérimentale</t>
+  </si>
+  <si>
+    <t>Nombre de répétitions pour le traitement expérimental</t>
+  </si>
+  <si>
+    <t>Combinaison des niveaux de facteurs appliqués (séparés par ";").</t>
+  </si>
+  <si>
+    <t>Nom ou code du traitement expérimental</t>
+  </si>
+  <si>
+    <t>Commentaires sur le traitement expérimental</t>
   </si>
 </sst>
 </file>
@@ -2310,8 +2310,8 @@
   <dimension ref="A1:AC128"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K141" sqref="K141"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.85546875" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2329,37 +2329,37 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>496</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>497</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>498</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>499</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>500</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>501</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>502</v>
-      </c>
       <c r="M1" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>388</v>
@@ -2374,19 +2374,19 @@
         <v>3</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>63</v>
@@ -2418,13 +2418,13 @@
         <v>164</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>71</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>165</v>
@@ -2444,22 +2444,22 @@
         <v>164</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>532</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>533</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>534</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>535</v>
-      </c>
       <c r="G3" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="N3" s="2">
         <v>1</v>
@@ -2473,16 +2473,16 @@
         <v>164</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>537</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>538</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>539</v>
-      </c>
       <c r="F4" s="2" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>5</v>
@@ -2539,16 +2539,16 @@
         <v>468</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>471</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>5</v>
@@ -2568,16 +2568,16 @@
         <v>468</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>71</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>5</v>
@@ -2597,25 +2597,25 @@
         <v>468</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="E9" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K9" s="2" t="s">
         <v>544</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>544</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>546</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>545</v>
       </c>
       <c r="N9" s="2">
         <v>3</v>
@@ -2629,16 +2629,16 @@
         <v>468</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E10" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>524</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>525</v>
-      </c>
       <c r="G10" s="2" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>5</v>
@@ -2655,16 +2655,16 @@
         <v>468</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>5</v>
@@ -2681,19 +2681,19 @@
         <v>468</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>5</v>
@@ -2713,16 +2713,16 @@
         <v>468</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>561</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>562</v>
+      </c>
+      <c r="G13" s="7" t="s">
         <v>565</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>567</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>566</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>569</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>5</v>
@@ -2731,7 +2731,7 @@
         <v>7</v>
       </c>
       <c r="X13" s="7" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="14" spans="1:29" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2742,25 +2742,25 @@
         <v>468</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>551</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>552</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>553</v>
       </c>
       <c r="G14" s="3">
         <v>1</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="N14" s="2">
         <v>9</v>
       </c>
       <c r="X14" s="2" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="15" spans="1:29" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -2771,10 +2771,10 @@
         <v>468</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>391</v>
@@ -2783,7 +2783,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:29" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>477</v>
       </c>
@@ -2808,11 +2808,14 @@
       <c r="H16" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="N16" s="2">
+        <v>1</v>
+      </c>
       <c r="O16" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:26" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>477</v>
       </c>
@@ -2837,16 +2840,19 @@
       <c r="K17" s="2" t="s">
         <v>143</v>
       </c>
+      <c r="N17" s="2">
+        <v>2</v>
+      </c>
       <c r="O17" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:26" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>477</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>128</v>
+        <v>555</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>401</v>
@@ -2858,7 +2864,7 @@
         <v>329</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>479</v>
+        <v>599</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>286</v>
@@ -2866,8 +2872,11 @@
       <c r="H18" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="19" spans="1:26" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N18" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>477</v>
       </c>
@@ -2889,8 +2898,11 @@
       <c r="H19" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="20" spans="1:26" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N19" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>477</v>
       </c>
@@ -2912,8 +2924,11 @@
       <c r="H20" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:26" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N20" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>477</v>
       </c>
@@ -2935,6 +2950,9 @@
       <c r="H21" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="N21" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="22" spans="1:26" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
@@ -2944,13 +2962,13 @@
         <v>247</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>5</v>
@@ -3037,7 +3055,7 @@
         <v>295</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="N25" s="2">
         <v>6</v>
@@ -3199,7 +3217,7 @@
         <v>5</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="S31" s="2" t="s">
         <v>9</v>
@@ -3236,16 +3254,16 @@
         <v>0</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="G33" s="7"/>
       <c r="H33" s="2" t="s">
@@ -3511,16 +3529,16 @@
         <v>326</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>236</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G41" s="2" t="s">
         <v>397</v>
@@ -3529,7 +3547,7 @@
         <v>5</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="N41" s="2">
         <v>3</v>
@@ -3552,13 +3570,13 @@
         <v>326</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="E42" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="F42" s="2" t="s">
         <v>507</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>508</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>327</v>
@@ -3587,16 +3605,16 @@
         <v>326</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="H43" s="2" t="s">
         <v>5</v>
@@ -3873,7 +3891,7 @@
         <v>279</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="N51" s="2">
         <v>8</v>
@@ -3926,7 +3944,7 @@
         <v>280</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="N52" s="2">
         <v>9</v>
@@ -4053,7 +4071,7 @@
         <v>273</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="N55" s="2">
         <v>13</v>
@@ -4085,7 +4103,7 @@
         <v>36</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G56" s="2" t="s">
         <v>37</v>
@@ -4097,7 +4115,7 @@
         <v>14</v>
       </c>
       <c r="S56" s="7" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="Z56" s="2" t="s">
         <v>298</v>
@@ -4117,7 +4135,7 @@
         <v>38</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="G57" s="2" t="s">
         <v>39</v>
@@ -4155,7 +4173,7 @@
         <v>283</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="N58" s="2">
         <v>16</v>
@@ -4193,7 +4211,7 @@
         <v>284</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="N59" s="2">
         <v>17</v>
@@ -4231,7 +4249,7 @@
         <v>274</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="N60" s="2">
         <v>18</v>
@@ -4298,7 +4316,7 @@
         <v>5</v>
       </c>
       <c r="K62" s="2" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="N62" s="2">
         <v>20</v>
@@ -4438,7 +4456,7 @@
         <v>272</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="N66" s="2">
         <v>24</v>
@@ -4473,7 +4491,7 @@
         <v>285</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="N67" s="2">
         <v>25</v>
@@ -4508,7 +4526,7 @@
         <v>0</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="N68" s="2">
         <v>26</v>
@@ -4549,7 +4567,7 @@
         <v>0</v>
       </c>
       <c r="H69" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="N69" s="2">
         <v>27</v>
@@ -4576,7 +4594,7 @@
         <v>477</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>423</v>
@@ -4617,13 +4635,13 @@
         <v>93</v>
       </c>
       <c r="C71" s="2" t="s">
+        <v>546</v>
+      </c>
+      <c r="E71" s="2" t="s">
         <v>547</v>
       </c>
-      <c r="E71" s="2" t="s">
-        <v>548</v>
-      </c>
       <c r="F71" s="2" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="H71" s="2" t="s">
         <v>5</v>
@@ -4707,7 +4725,7 @@
         <v>289</v>
       </c>
       <c r="H74" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="Z74" s="2" t="s">
         <v>245</v>
@@ -4736,7 +4754,7 @@
         <v>290</v>
       </c>
       <c r="H75" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="76" spans="1:29" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -4831,16 +4849,16 @@
         <v>93</v>
       </c>
       <c r="C79" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="E79" s="2" t="s">
         <v>490</v>
       </c>
-      <c r="E79" s="2" t="s">
+      <c r="F79" s="2" t="s">
         <v>491</v>
       </c>
-      <c r="F79" s="2" t="s">
+      <c r="G79" s="2" t="s">
         <v>492</v>
-      </c>
-      <c r="G79" s="2" t="s">
-        <v>493</v>
       </c>
       <c r="H79" s="2" t="s">
         <v>5</v>
@@ -4849,7 +4867,7 @@
         <v>2</v>
       </c>
       <c r="X79" s="7" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="80" spans="1:29" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -4933,7 +4951,7 @@
         <v>307</v>
       </c>
       <c r="G82" s="2" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="H82" s="2" t="s">
         <v>5</v>
@@ -5249,13 +5267,13 @@
         <v>166</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="H93" s="2" t="s">
         <v>5</v>
@@ -5510,7 +5528,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="101" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:27" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>477</v>
       </c>
@@ -5518,19 +5536,19 @@
         <v>108</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="H101" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="102" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:27" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>477</v>
       </c>
@@ -5559,7 +5577,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="103" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:27" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>477</v>
       </c>
@@ -5579,7 +5597,7 @@
         <v>275</v>
       </c>
       <c r="H103" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="O103" s="2">
         <v>2</v>
@@ -5588,7 +5606,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="104" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:27" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>477</v>
       </c>
@@ -5626,7 +5644,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="105" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:27" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>477</v>
       </c>
@@ -5661,7 +5679,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="106" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:27" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>477</v>
       </c>
@@ -5684,13 +5702,13 @@
         <v>276</v>
       </c>
       <c r="H106" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="O106" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="107" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:27" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>477</v>
       </c>
@@ -5713,13 +5731,13 @@
         <v>277</v>
       </c>
       <c r="H107" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="O107" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="108" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:27" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>477</v>
       </c>
@@ -5739,7 +5757,7 @@
         <v>278</v>
       </c>
       <c r="H108" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="O108" s="2">
         <v>2</v>
@@ -5751,7 +5769,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="109" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:27" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>477</v>
       </c>
@@ -5959,7 +5977,7 @@
         <v>293</v>
       </c>
       <c r="H116" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="P116" s="2">
         <v>0</v>
@@ -6049,38 +6067,41 @@
         <v>301</v>
       </c>
     </row>
-    <row r="120" spans="1:26" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>477</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="E120" s="2" t="s">
         <v>234</v>
       </c>
       <c r="F120" s="2" t="s">
-        <v>556</v>
+        <v>601</v>
       </c>
       <c r="G120" s="2" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="H120" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="121" spans="1:26" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N120" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>477</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="C121" s="2" t="s">
         <v>402</v>
@@ -6092,39 +6113,45 @@
         <v>328</v>
       </c>
       <c r="F121" s="2" t="s">
-        <v>561</v>
+        <v>600</v>
       </c>
       <c r="G121" s="2" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="H121" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="122" spans="1:26" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N121" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>477</v>
       </c>
       <c r="B122" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="D122" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="E122" s="2" t="s">
         <v>557</v>
       </c>
-      <c r="C122" s="2" t="s">
-        <v>558</v>
-      </c>
-      <c r="D122" s="2" t="s">
-        <v>558</v>
-      </c>
-      <c r="E122" s="2" t="s">
-        <v>559</v>
-      </c>
       <c r="F122" s="2" t="s">
-        <v>560</v>
+        <v>602</v>
       </c>
       <c r="G122" s="2" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="H122" s="2" t="s">
         <v>5</v>
+      </c>
+      <c r="N122" s="2">
+        <v>4</v>
       </c>
     </row>
     <row r="123" spans="1:26" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -6135,16 +6162,16 @@
         <v>468</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="E123" s="2" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="F123" s="2" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="G123" s="2" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="H123" s="2" t="s">
         <v>5</v>
@@ -6158,19 +6185,19 @@
         <v>477</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="C124" s="12" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="D124" s="12" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="E124" s="2" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="F124" s="2" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="H124" s="2" t="s">
         <v>5</v>
@@ -6181,16 +6208,16 @@
         <v>477</v>
       </c>
       <c r="B125" s="2" t="s">
+        <v>574</v>
+      </c>
+      <c r="C125" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="E125" s="2" t="s">
         <v>578</v>
       </c>
-      <c r="C125" s="2" t="s">
-        <v>581</v>
-      </c>
-      <c r="E125" s="2" t="s">
-        <v>582</v>
-      </c>
       <c r="F125" s="2" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="H125" s="2" t="s">
         <v>5</v>
@@ -6201,16 +6228,16 @@
         <v>477</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="E126" s="2" t="s">
         <v>94</v>
       </c>
       <c r="F126" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="G126" s="3" t="s">
         <v>288</v>
@@ -6224,22 +6251,22 @@
         <v>477</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="E127" s="2" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="F127" s="2" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="G127" s="3" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="H127" s="2" t="s">
         <v>5</v>
@@ -6253,22 +6280,22 @@
         <v>477</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="E128" s="2" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
       <c r="F128" s="2" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="G128" s="3" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="H128" s="2" t="s">
         <v>5</v>
@@ -6278,7 +6305,8 @@
   <autoFilter ref="B1:AC128" xr:uid="{FB13ADFC-DCBE-45B8-93DC-72D8CCE37DD2}">
     <filterColumn colId="0">
       <filters>
-        <filter val="soil"/>
+        <filter val="design"/>
+        <filter val="treatment"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
minor update with required fields
</commit_message>
<xml_diff>
--- a/experimental_context_description.xlsx
+++ b/experimental_context_description.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vignevin-my.sharepoint.com/personal/xavier_delpuech_vignevin_com/Documents/AgricultureNumerique/ProjetsEnCours/VITISDATACROP/05_TRAVAIL_EN_COURS/WP1.1 Harmonisation/Experimentation/vitisdatacrop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="270" documentId="13_ncr:1_{7E65C6BA-C87A-4619-9764-C45083FA781A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4052FCD4-2511-4219-8825-9A8B0B11474D}"/>
+  <xr:revisionPtr revIDLastSave="276" documentId="13_ncr:1_{7E65C6BA-C87A-4619-9764-C45083FA781A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3D56D5DF-414F-419F-B9AE-B9BFB67716A5}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1AE09EEA-C0A3-42DC-AFC7-BA79A75A8C50}"/>
   </bookViews>
@@ -2378,9 +2378,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB13ADFC-DCBE-45B8-93DC-72D8CCE37DD2}">
   <dimension ref="A1:AC133"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J108" sqref="J108"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.85546875" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3402,6 +3402,9 @@
       <c r="H35" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="M35" s="2">
+        <v>1</v>
+      </c>
       <c r="N35" s="2">
         <v>2</v>
       </c>
@@ -4798,6 +4801,9 @@
       </c>
       <c r="H74" s="2" t="s">
         <v>5</v>
+      </c>
+      <c r="M74" s="2">
+        <v>1</v>
       </c>
       <c r="N74" s="2">
         <v>2</v>

</xml_diff>

<commit_message>
name correction for data_dictionary and field_wine_area
</commit_message>
<xml_diff>
--- a/experimental_context_description.xlsx
+++ b/experimental_context_description.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vignevin-my.sharepoint.com/personal/xavier_delpuech_vignevin_com/Documents/AgricultureNumerique/ProjetsEnCours/VITISDATACROP/05_TRAVAIL_EN_COURS/WP1.1 Harmonisation/Experimentation/vitisdatacrop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="276" documentId="13_ncr:1_{7E65C6BA-C87A-4619-9764-C45083FA781A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3D56D5DF-414F-419F-B9AE-B9BFB67716A5}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{D16C2F42-B43A-4C59-A199-3C52AD3D54E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{74FBF631-49AD-4D75-A5A8-E183C63751DC}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1AE09EEA-C0A3-42DC-AFC7-BA79A75A8C50}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1AE09EEA-C0A3-42DC-AFC7-BA79A75A8C50}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$B$1:$AC$133</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$B$1:$AC$134</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1123" uniqueCount="627">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1132" uniqueCount="631">
   <si>
     <t>experimentation</t>
   </si>
@@ -1066,9 +1066,6 @@
     <t>https://www.legifrance.gouv.fr/codes/section_lc/LEGITEXT000006071367/LEGISCTA000036441436/2020-07-02/?anchor=LEGIARTI000036441438#LEGIARTI000036441438</t>
   </si>
   <si>
-    <t>Alsace Est,Aquitaine,Bourgogne-Beaujolais-Savoie-Jura,Champagne,Charentes-Cognac,Corse,Languedoc-Roussillon,Sud-Ouest,Val-de-Loire-Centre, Vallée-du-Rhône-Provence</t>
-  </si>
-  <si>
     <t>AAAA</t>
   </si>
   <si>
@@ -1306,9 +1303,6 @@
     <t>field_insee_commune</t>
   </si>
   <si>
-    <t>field_bassin</t>
-  </si>
-  <si>
     <t>field_previous_crop</t>
   </si>
   <si>
@@ -1420,9 +1414,6 @@
     <t>fertiliz_app_name</t>
   </si>
   <si>
-    <t>data_dictionnary</t>
-  </si>
-  <si>
     <t>data_file_name</t>
   </si>
   <si>
@@ -1925,6 +1916,27 @@
   </si>
   <si>
     <t>GARP:2069;GARP:2051</t>
+  </si>
+  <si>
+    <t>Alsace Est,Aquitaine,Bourgogne-Beaujolais-Savoie-Jura,Champagne,Charentes-Cognac,Corse,Languedoc-Roussillon,Sud-Ouest,Val-de-Loire-Centre,Vallée-du-Rhône-Provence</t>
+  </si>
+  <si>
+    <t>tr_field</t>
+  </si>
+  <si>
+    <t>Parcelle sur laquelle est mis en place le traitement expérimental</t>
+  </si>
+  <si>
+    <t>Le Mas</t>
+  </si>
+  <si>
+    <t>https://cropontology.org/term/CO_356:1000166</t>
+  </si>
+  <si>
+    <t>data_dictionary</t>
+  </si>
+  <si>
+    <t>field_wine_area</t>
   </si>
 </sst>
 </file>
@@ -1934,7 +1946,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1996,6 +2008,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF212121"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2020,7 +2038,7 @@
     <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2059,6 +2077,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -2376,16 +2395,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB13ADFC-DCBE-45B8-93DC-72D8CCE37DD2}">
-  <dimension ref="A1:AC133"/>
+  <dimension ref="A1:AC134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.85546875" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="14.85546875" style="2"/>
+    <col min="1" max="1" width="14.85546875" style="2"/>
+    <col min="2" max="2" width="23.5703125" style="2" customWidth="1"/>
     <col min="3" max="3" width="32.140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="26.140625" style="2" customWidth="1"/>
     <col min="5" max="5" width="36.7109375" style="2" customWidth="1"/>
@@ -2398,46 +2418,46 @@
   <sheetData>
     <row r="1" spans="1:29" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>482</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>483</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>484</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>485</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>487</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>488</v>
-      </c>
       <c r="M1" s="1" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>308</v>
@@ -2449,19 +2469,19 @@
         <v>3</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>63</v>
@@ -2487,19 +2507,19 @@
     </row>
     <row r="2" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>161</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>71</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>162</v>
@@ -2513,28 +2533,28 @@
     </row>
     <row r="3" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>161</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="N3" s="2">
         <v>1</v>
@@ -2542,22 +2562,22 @@
     </row>
     <row r="4" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>161</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>518</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>519</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>521</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>522</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>526</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>524</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>5</v>
@@ -2568,19 +2588,19 @@
     </row>
     <row r="5" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>458</v>
+        <v>629</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>5</v>
@@ -2588,19 +2608,19 @@
     </row>
     <row r="6" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>458</v>
+        <v>629</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>5</v>
@@ -2608,22 +2628,22 @@
     </row>
     <row r="7" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>629</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>539</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>458</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>542</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>461</v>
-      </c>
       <c r="F7" s="2" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>5</v>
@@ -2637,22 +2657,22 @@
     </row>
     <row r="8" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>458</v>
+        <v>629</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>71</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>5</v>
@@ -2666,31 +2686,31 @@
     </row>
     <row r="9" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>458</v>
+        <v>629</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="N9" s="2">
         <v>3</v>
@@ -2698,22 +2718,22 @@
     </row>
     <row r="10" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>458</v>
+        <v>629</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="E10" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>508</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>509</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>511</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>5</v>
@@ -2724,22 +2744,22 @@
     </row>
     <row r="11" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>458</v>
+        <v>629</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>5</v>
@@ -2750,28 +2770,28 @@
     </row>
     <row r="12" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>458</v>
+        <v>629</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>574</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>577</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="H12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K12" s="2" t="s">
         <v>578</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>579</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>580</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>581</v>
       </c>
       <c r="N12" s="2">
         <v>7</v>
@@ -2779,25 +2799,25 @@
     </row>
     <row r="13" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>458</v>
+        <v>629</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>5</v>
@@ -2811,22 +2831,22 @@
     </row>
     <row r="14" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>458</v>
+        <v>629</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>5</v>
@@ -2835,53 +2855,53 @@
         <v>8</v>
       </c>
       <c r="X14" s="7" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="15" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>458</v>
+        <v>629</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="G15" s="3">
         <v>1</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="N15" s="2">
         <v>10</v>
       </c>
       <c r="X15" s="2" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
     </row>
     <row r="16" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>458</v>
+        <v>629</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>504</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>507</v>
-      </c>
       <c r="F16" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>5</v>
@@ -2889,7 +2909,7 @@
     </row>
     <row r="17" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>126</v>
@@ -2898,7 +2918,7 @@
         <v>127</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>128</v>
@@ -2921,7 +2941,7 @@
     </row>
     <row r="18" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>126</v>
@@ -2942,7 +2962,7 @@
         <v>5</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="N18" s="2">
         <v>2</v>
@@ -2953,22 +2973,22 @@
     </row>
     <row r="19" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>320</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>279</v>
@@ -2977,12 +2997,12 @@
         <v>32</v>
       </c>
       <c r="N19" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>126</v>
@@ -3008,7 +3028,7 @@
     </row>
     <row r="21" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>126</v>
@@ -3034,7 +3054,7 @@
     </row>
     <row r="22" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>126</v>
@@ -3060,19 +3080,22 @@
     </row>
     <row r="23" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>240</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>574</v>
+        <v>571</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>627</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>5</v>
@@ -3083,7 +3106,7 @@
     </row>
     <row r="24" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>240</v>
@@ -3112,7 +3135,7 @@
     </row>
     <row r="25" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>240</v>
@@ -3141,7 +3164,7 @@
     </row>
     <row r="26" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>240</v>
@@ -3159,7 +3182,7 @@
         <v>288</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="N26" s="2">
         <v>6</v>
@@ -3173,7 +3196,7 @@
     </row>
     <row r="27" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>240</v>
@@ -3202,7 +3225,7 @@
     </row>
     <row r="28" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>240</v>
@@ -3228,7 +3251,7 @@
     </row>
     <row r="29" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>240</v>
@@ -3254,22 +3277,22 @@
     </row>
     <row r="30" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="B30" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="E30" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="F30" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="G30" s="2" t="s">
         <v>365</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>366</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>5</v>
@@ -3277,22 +3300,22 @@
     </row>
     <row r="31" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C31" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="F31" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="F31" s="2" t="s">
-        <v>369</v>
-      </c>
       <c r="G31" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>5</v>
@@ -3300,28 +3323,28 @@
     </row>
     <row r="32" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>372</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J32" s="2" t="s">
         <v>468</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>362</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>370</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>371</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>372</v>
-      </c>
-      <c r="G32" s="9" t="s">
-        <v>373</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J32" s="2" t="s">
-        <v>471</v>
       </c>
       <c r="S32" s="2" t="s">
         <v>9</v>
@@ -3329,22 +3352,22 @@
     </row>
     <row r="33" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>5</v>
@@ -3352,22 +3375,22 @@
     </row>
     <row r="34" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="G34" s="7"/>
       <c r="H34" s="2" t="s">
@@ -3379,16 +3402,16 @@
     </row>
     <row r="35" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>87</v>
@@ -3417,7 +3440,7 @@
     </row>
     <row r="36" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>0</v>
@@ -3458,7 +3481,7 @@
     </row>
     <row r="37" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>0</v>
@@ -3499,16 +3522,16 @@
     </row>
     <row r="38" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>70</v>
@@ -3534,16 +3557,16 @@
     </row>
     <row r="39" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>71</v>
@@ -3566,7 +3589,7 @@
     </row>
     <row r="40" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>0</v>
@@ -3595,16 +3618,16 @@
     </row>
     <row r="41" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>74</v>
@@ -3630,31 +3653,31 @@
     </row>
     <row r="42" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B42" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>596</v>
+      </c>
+      <c r="F42" s="2" t="s">
         <v>595</v>
       </c>
-      <c r="C42" s="2" t="s">
-        <v>568</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>568</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>599</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>598</v>
-      </c>
       <c r="G42" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="H42" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="N42" s="2">
         <v>3</v>
@@ -3671,19 +3694,19 @@
     </row>
     <row r="43" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>319</v>
@@ -3706,22 +3729,22 @@
     </row>
     <row r="44" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="E44" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="F44" s="2" t="s">
         <v>494</v>
       </c>
-      <c r="F44" s="2" t="s">
-        <v>497</v>
-      </c>
       <c r="G44" s="2" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="H44" s="2" t="s">
         <v>5</v>
@@ -3735,19 +3758,19 @@
     </row>
     <row r="45" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="H45" s="2" t="s">
         <v>5</v>
@@ -3755,25 +3778,25 @@
     </row>
     <row r="46" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E46" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="F46" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="F46" s="2" t="s">
+      <c r="G46" s="7" t="s">
         <v>408</v>
-      </c>
-      <c r="G46" s="7" t="s">
-        <v>409</v>
       </c>
       <c r="H46" s="2" t="s">
         <v>5</v>
@@ -3787,13 +3810,13 @@
     </row>
     <row r="47" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>33</v>
@@ -3816,16 +3839,16 @@
     </row>
     <row r="48" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>19</v>
@@ -3848,16 +3871,16 @@
     </row>
     <row r="49" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>22</v>
@@ -3886,13 +3909,13 @@
     </row>
     <row r="50" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>158</v>
@@ -3924,22 +3947,22 @@
     </row>
     <row r="51" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>264</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="H51" s="2" t="s">
         <v>5</v>
@@ -3951,7 +3974,7 @@
         <v>3</v>
       </c>
       <c r="X51" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="Z51" s="2" t="s">
         <v>262</v>
@@ -3959,13 +3982,13 @@
     </row>
     <row r="52" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>420</v>
+        <v>630</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>27</v>
@@ -3980,7 +4003,7 @@
         <v>5</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>340</v>
+        <v>624</v>
       </c>
       <c r="N52" s="2">
         <v>7</v>
@@ -3989,7 +4012,7 @@
         <v>3</v>
       </c>
       <c r="W52" s="3" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="X52" s="7" t="s">
         <v>339</v>
@@ -3997,16 +4020,16 @@
     </row>
     <row r="53" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>85</v>
@@ -4018,7 +4041,7 @@
         <v>272</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="N53" s="2">
         <v>8</v>
@@ -4050,16 +4073,16 @@
     </row>
     <row r="54" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>86</v>
@@ -4071,7 +4094,7 @@
         <v>273</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="N54" s="2">
         <v>9</v>
@@ -4103,13 +4126,13 @@
     </row>
     <row r="55" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B55" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="C55" s="2" t="s">
         <v>416</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>417</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>334</v>
@@ -4136,22 +4159,22 @@
         <v>335</v>
       </c>
       <c r="X55" s="13" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="AC55" s="7"/>
     </row>
     <row r="56" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>30</v>
@@ -4166,7 +4189,7 @@
         <v>5</v>
       </c>
       <c r="L56" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="N56" s="2">
         <v>11</v>
@@ -4180,16 +4203,16 @@
     </row>
     <row r="57" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>182</v>
@@ -4201,7 +4224,7 @@
         <v>266</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="N57" s="2">
         <v>13</v>
@@ -4218,22 +4241,22 @@
     </row>
     <row r="58" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>36</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="G58" s="2" t="s">
         <v>37</v>
@@ -4245,10 +4268,10 @@
         <v>14</v>
       </c>
       <c r="S58" s="7" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="X58" s="13" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="Z58" s="2" t="s">
         <v>291</v>
@@ -4256,19 +4279,19 @@
     </row>
     <row r="59" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>38</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="G59" s="2" t="s">
         <v>39</v>
@@ -4280,7 +4303,7 @@
         <v>15</v>
       </c>
       <c r="X59" s="7" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="Z59" s="2" t="s">
         <v>291</v>
@@ -4288,68 +4311,68 @@
     </row>
     <row r="60" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C60" s="2" t="s">
+        <v>585</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>610</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>612</v>
+      </c>
+      <c r="G60" s="7" t="s">
         <v>588</v>
       </c>
-      <c r="E60" s="2" t="s">
-        <v>613</v>
-      </c>
-      <c r="F60" s="2" t="s">
-        <v>615</v>
-      </c>
-      <c r="G60" s="7" t="s">
-        <v>591</v>
-      </c>
       <c r="H60" s="2" t="s">
         <v>5</v>
       </c>
       <c r="X60" s="2" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
     </row>
     <row r="61" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="G61" s="7" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="H61" s="2" t="s">
         <v>5</v>
       </c>
       <c r="X61" s="2" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
     </row>
     <row r="62" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>40</v>
@@ -4361,7 +4384,7 @@
         <v>276</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="N62" s="2">
         <v>16</v>
@@ -4378,16 +4401,16 @@
     </row>
     <row r="63" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>46</v>
@@ -4399,7 +4422,7 @@
         <v>277</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="N63" s="2">
         <v>17</v>
@@ -4416,16 +4439,16 @@
     </row>
     <row r="64" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>184</v>
@@ -4437,7 +4460,7 @@
         <v>267</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="N64" s="2">
         <v>18</v>
@@ -4445,16 +4468,20 @@
       <c r="Z64" s="2" t="s">
         <v>262</v>
       </c>
+      <c r="AB64" s="14"/>
+      <c r="AC64" s="14" t="s">
+        <v>628</v>
+      </c>
     </row>
     <row r="65" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>47</v>
@@ -4483,13 +4510,13 @@
     </row>
     <row r="66" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>48</v>
@@ -4504,7 +4531,7 @@
         <v>5</v>
       </c>
       <c r="K66" s="2" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="N66" s="2">
         <v>20</v>
@@ -4518,16 +4545,16 @@
     </row>
     <row r="67" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>11</v>
@@ -4556,13 +4583,13 @@
     </row>
     <row r="68" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>53</v>
@@ -4591,13 +4618,13 @@
     </row>
     <row r="69" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>54</v>
@@ -4626,13 +4653,13 @@
     </row>
     <row r="70" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>55</v>
@@ -4644,7 +4671,7 @@
         <v>265</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="N70" s="2">
         <v>24</v>
@@ -4658,16 +4685,16 @@
     </row>
     <row r="71" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>49</v>
@@ -4679,7 +4706,7 @@
         <v>278</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="N71" s="2">
         <v>25</v>
@@ -4693,28 +4720,28 @@
     </row>
     <row r="72" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>186</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="G72" s="2">
         <v>0</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="N72" s="2">
         <v>26</v>
@@ -4734,28 +4761,28 @@
     </row>
     <row r="73" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>50</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="G73" s="11">
         <v>0</v>
       </c>
       <c r="H73" s="2" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="N73" s="2">
         <v>27</v>
@@ -4779,16 +4806,16 @@
     </row>
     <row r="74" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>20</v>
@@ -4820,19 +4847,19 @@
     </row>
     <row r="75" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="H75" s="2" t="s">
         <v>5</v>
@@ -4840,19 +4867,19 @@
     </row>
     <row r="76" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="G76" s="3" t="s">
         <v>281</v>
@@ -4861,7 +4888,7 @@
         <v>5</v>
       </c>
       <c r="L76" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="Z76" s="2" t="s">
         <v>238</v>
@@ -4869,42 +4896,42 @@
     </row>
     <row r="77" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C77" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="F77" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="E77" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="F77" s="2" t="s">
-        <v>347</v>
-      </c>
       <c r="G77" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H77" s="2" t="s">
         <v>5</v>
       </c>
       <c r="L77" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="78" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>95</v>
@@ -4916,7 +4943,7 @@
         <v>282</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="Z78" s="2" t="s">
         <v>238</v>
@@ -4924,16 +4951,16 @@
     </row>
     <row r="79" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>96</v>
@@ -4945,12 +4972,12 @@
         <v>283</v>
       </c>
       <c r="H79" s="2" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
     </row>
     <row r="80" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>93</v>
@@ -4976,7 +5003,7 @@
     </row>
     <row r="81" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B81" s="2" t="s">
         <v>93</v>
@@ -4985,7 +5012,7 @@
         <v>104</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>98</v>
@@ -5005,16 +5032,16 @@
     </row>
     <row r="82" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>189</v>
@@ -5034,22 +5061,22 @@
     </row>
     <row r="83" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C83" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="F83" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="G83" s="2" t="s">
         <v>477</v>
-      </c>
-      <c r="E83" s="2" t="s">
-        <v>478</v>
-      </c>
-      <c r="F83" s="2" t="s">
-        <v>479</v>
-      </c>
-      <c r="G83" s="2" t="s">
-        <v>480</v>
       </c>
       <c r="H83" s="2" t="s">
         <v>5</v>
@@ -5058,33 +5085,33 @@
         <v>2</v>
       </c>
       <c r="X83" s="7" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
     </row>
     <row r="84" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E84" s="2" t="s">
         <v>51</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G84" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H84" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K84" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="O84" s="2">
         <v>2</v>
@@ -5095,13 +5122,13 @@
     </row>
     <row r="85" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E85" s="2" t="s">
         <v>52</v>
@@ -5110,13 +5137,13 @@
         <v>301</v>
       </c>
       <c r="G85" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H85" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K85" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="O85" s="2">
         <v>2</v>
@@ -5127,13 +5154,13 @@
     </row>
     <row r="86" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>299</v>
@@ -5142,7 +5169,7 @@
         <v>300</v>
       </c>
       <c r="G86" s="2" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="H86" s="2" t="s">
         <v>5</v>
@@ -5156,22 +5183,22 @@
     </row>
     <row r="87" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C87" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="E87" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="E87" s="2" t="s">
+      <c r="F87" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="G87" s="2" t="s">
         <v>356</v>
-      </c>
-      <c r="F87" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="G87" s="2" t="s">
-        <v>357</v>
       </c>
       <c r="H87" s="2" t="s">
         <v>5</v>
@@ -5179,25 +5206,25 @@
     </row>
     <row r="88" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B88" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="C88" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="C88" s="2" t="s">
+      <c r="D88" s="2" t="s">
         <v>396</v>
-      </c>
-      <c r="D88" s="2" t="s">
-        <v>397</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>72</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="G88" s="5" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="H88" s="2" t="s">
         <v>5</v>
@@ -5214,25 +5241,25 @@
     </row>
     <row r="89" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>73</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="G89" s="5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="H89" s="2" t="s">
         <v>5</v>
@@ -5252,31 +5279,31 @@
     </row>
     <row r="90" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C90" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="E90" s="2" t="s">
         <v>399</v>
       </c>
-      <c r="D90" s="2" t="s">
-        <v>399</v>
-      </c>
-      <c r="E90" s="2" t="s">
-        <v>400</v>
-      </c>
       <c r="F90" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="G90" s="5" t="s">
         <v>403</v>
       </c>
-      <c r="G90" s="5" t="s">
-        <v>404</v>
-      </c>
       <c r="H90" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K90" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="O90" s="2">
         <v>2</v>
@@ -5284,16 +5311,16 @@
     </row>
     <row r="91" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>321</v>
@@ -5313,13 +5340,13 @@
     </row>
     <row r="92" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>225</v>
@@ -5342,13 +5369,13 @@
     </row>
     <row r="93" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="B93" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="C93" s="2" t="s">
         <v>434</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>436</v>
       </c>
       <c r="E93" s="2" t="s">
         <v>324</v>
@@ -5371,13 +5398,13 @@
     </row>
     <row r="94" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>325</v>
@@ -5400,13 +5427,13 @@
     </row>
     <row r="95" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="E95" s="2" t="s">
         <v>226</v>
@@ -5426,13 +5453,13 @@
     </row>
     <row r="96" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="E96" s="2" t="s">
         <v>228</v>
@@ -5452,19 +5479,19 @@
     </row>
     <row r="97" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>163</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="H97" s="2" t="s">
         <v>5</v>
@@ -5475,7 +5502,7 @@
     </row>
     <row r="98" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B98" s="2" t="s">
         <v>163</v>
@@ -5511,7 +5538,7 @@
     </row>
     <row r="99" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B99" s="2" t="s">
         <v>163</v>
@@ -5543,7 +5570,7 @@
     </row>
     <row r="100" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B100" s="2" t="s">
         <v>163</v>
@@ -5581,7 +5608,7 @@
     </row>
     <row r="101" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>163</v>
@@ -5619,7 +5646,7 @@
     </row>
     <row r="102" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B102" s="2" t="s">
         <v>163</v>
@@ -5651,7 +5678,7 @@
     </row>
     <row r="103" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B103" s="2" t="s">
         <v>163</v>
@@ -5686,25 +5713,25 @@
     </row>
     <row r="104" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B104" s="2" t="s">
         <v>163</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="G104" s="2" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="H104" s="2" t="s">
         <v>5</v>
@@ -5721,22 +5748,22 @@
     </row>
     <row r="105" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B105" s="2" t="s">
         <v>163</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="G105" s="2" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="H105" s="2" t="s">
         <v>5</v>
@@ -5750,19 +5777,19 @@
     </row>
     <row r="106" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B106" s="2" t="s">
         <v>108</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="H106" s="2" t="s">
         <v>5</v>
@@ -5770,7 +5797,7 @@
     </row>
     <row r="107" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B107" s="2" t="s">
         <v>108</v>
@@ -5799,7 +5826,7 @@
     </row>
     <row r="108" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B108" s="2" t="s">
         <v>108</v>
@@ -5817,7 +5844,7 @@
         <v>268</v>
       </c>
       <c r="H108" s="2" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="O108" s="2">
         <v>2</v>
@@ -5828,22 +5855,22 @@
     </row>
     <row r="109" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B109" s="2" t="s">
         <v>108</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="E109" s="2" t="s">
         <v>111</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="G109" s="2" t="s">
         <v>123</v>
@@ -5852,7 +5879,7 @@
         <v>5</v>
       </c>
       <c r="K109" s="2" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="O109" s="2">
         <v>2</v>
@@ -5866,7 +5893,7 @@
     </row>
     <row r="110" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B110" s="2" t="s">
         <v>108</v>
@@ -5893,7 +5920,7 @@
         <v>2</v>
       </c>
       <c r="W110" s="3" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="Z110" s="2" t="s">
         <v>294</v>
@@ -5901,28 +5928,28 @@
     </row>
     <row r="111" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B111" s="2" t="s">
         <v>108</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="E111" s="2" t="s">
         <v>113</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="G111" s="3" t="s">
         <v>269</v>
       </c>
       <c r="H111" s="2" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="O111" s="2">
         <v>2</v>
@@ -5930,16 +5957,16 @@
     </row>
     <row r="112" spans="1:28" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B112" s="2" t="s">
         <v>108</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="E112" s="2" t="s">
         <v>114</v>
@@ -5951,7 +5978,7 @@
         <v>270</v>
       </c>
       <c r="H112" s="2" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="O112" s="2">
         <v>2</v>
@@ -5959,7 +5986,7 @@
     </row>
     <row r="113" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B113" s="2" t="s">
         <v>108</v>
@@ -5977,7 +6004,7 @@
         <v>271</v>
       </c>
       <c r="H113" s="2" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="O113" s="2">
         <v>2</v>
@@ -5991,22 +6018,22 @@
     </row>
     <row r="114" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B114" s="2" t="s">
         <v>108</v>
       </c>
       <c r="C114" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="E114" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="F114" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="E114" s="2" t="s">
-        <v>356</v>
-      </c>
-      <c r="F114" s="2" t="s">
+      <c r="G114" s="2" t="s">
         <v>360</v>
-      </c>
-      <c r="G114" s="2" t="s">
-        <v>361</v>
       </c>
       <c r="H114" s="2" t="s">
         <v>5</v>
@@ -6014,7 +6041,7 @@
     </row>
     <row r="115" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="B115" s="2" t="s">
         <v>193</v>
@@ -6040,7 +6067,7 @@
     </row>
     <row r="116" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="B116" s="2" t="s">
         <v>193</v>
@@ -6069,7 +6096,7 @@
     </row>
     <row r="117" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="B117" s="2" t="s">
         <v>193</v>
@@ -6098,7 +6125,7 @@
     </row>
     <row r="118" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="B118" s="2" t="s">
         <v>193</v>
@@ -6124,7 +6151,7 @@
     </row>
     <row r="119" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="B119" s="2" t="s">
         <v>193</v>
@@ -6153,7 +6180,7 @@
     </row>
     <row r="120" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="B120" s="2" t="s">
         <v>193</v>
@@ -6179,7 +6206,7 @@
     </row>
     <row r="121" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="B121" s="2" t="s">
         <v>193</v>
@@ -6197,7 +6224,7 @@
         <v>286</v>
       </c>
       <c r="H121" s="2" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="P121" s="2">
         <v>0</v>
@@ -6208,7 +6235,7 @@
     </row>
     <row r="122" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="B122" s="2" t="s">
         <v>193</v>
@@ -6237,7 +6264,7 @@
     </row>
     <row r="123" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="B123" s="2" t="s">
         <v>193</v>
@@ -6263,7 +6290,7 @@
     </row>
     <row r="124" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="B124" s="2" t="s">
         <v>193</v>
@@ -6289,240 +6316,266 @@
     </row>
     <row r="125" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="E125" s="2" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="F125" s="2" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="G125" s="2" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="H125" s="2" t="s">
         <v>5</v>
       </c>
       <c r="N125" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="126" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E126" s="2" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="F126" s="2" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="G126" s="2" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="H126" s="2" t="s">
         <v>5</v>
       </c>
       <c r="N126" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="127" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="E127" s="2" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="F127" s="2" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="G127" s="2" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="H127" s="2" t="s">
         <v>5</v>
       </c>
       <c r="N127" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="128" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>458</v>
+        <v>598</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>547</v>
+        <v>625</v>
       </c>
       <c r="E128" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="F128" s="2" t="s">
+        <v>626</v>
+      </c>
+      <c r="G128" s="2" t="s">
+        <v>627</v>
+      </c>
+      <c r="H128" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N128" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>629</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="E129" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="F129" s="2" t="s">
+        <v>614</v>
+      </c>
+      <c r="G129" s="2" t="s">
+        <v>542</v>
+      </c>
+      <c r="H129" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N129" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="130" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="B130" s="2" t="s">
         <v>548</v>
       </c>
-      <c r="F128" s="2" t="s">
-        <v>617</v>
-      </c>
-      <c r="G128" s="2" t="s">
-        <v>545</v>
-      </c>
-      <c r="H128" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="N128" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="129" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="2" t="s">
-        <v>467</v>
-      </c>
-      <c r="B129" s="2" t="s">
+      <c r="C130" s="12" t="s">
+        <v>535</v>
+      </c>
+      <c r="D130" s="12" t="s">
+        <v>535</v>
+      </c>
+      <c r="E130" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="F130" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="H130" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="131" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="C131" s="2" t="s">
         <v>551</v>
       </c>
-      <c r="C129" s="12" t="s">
-        <v>538</v>
-      </c>
-      <c r="D129" s="12" t="s">
-        <v>538</v>
-      </c>
-      <c r="E129" s="2" t="s">
+      <c r="E131" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="F129" s="2" t="s">
+      <c r="F131" s="2" t="s">
         <v>553</v>
       </c>
-      <c r="H129" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="130" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="2" t="s">
-        <v>467</v>
-      </c>
-      <c r="B130" s="2" t="s">
-        <v>551</v>
-      </c>
-      <c r="C130" s="2" t="s">
+      <c r="H131" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="132" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>564</v>
+      </c>
+      <c r="C132" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="E130" s="2" t="s">
+      <c r="E132" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F132" s="2" t="s">
         <v>555</v>
       </c>
-      <c r="F130" s="2" t="s">
+      <c r="G132" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="H132" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="133" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="C133" s="2" t="s">
         <v>556</v>
       </c>
-      <c r="H130" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="131" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="2" t="s">
-        <v>467</v>
-      </c>
-      <c r="B131" s="2" t="s">
-        <v>567</v>
-      </c>
-      <c r="C131" s="2" t="s">
+      <c r="D133" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="E133" s="2" t="s">
         <v>557</v>
       </c>
-      <c r="E131" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="F131" s="2" t="s">
+      <c r="F133" s="2" t="s">
         <v>558</v>
       </c>
-      <c r="G131" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="H131" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="132" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="2" t="s">
-        <v>467</v>
-      </c>
-      <c r="B132" s="2" t="s">
-        <v>551</v>
-      </c>
-      <c r="C132" s="2" t="s">
+      <c r="G133" s="3" t="s">
         <v>559</v>
       </c>
-      <c r="D132" s="2" t="s">
-        <v>559</v>
-      </c>
-      <c r="E132" s="2" t="s">
+      <c r="H133" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J133" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="134" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="C134" s="2" t="s">
         <v>560</v>
       </c>
-      <c r="F132" s="2" t="s">
+      <c r="D134" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="E134" s="2" t="s">
         <v>561</v>
       </c>
-      <c r="G132" s="3" t="s">
+      <c r="F134" s="2" t="s">
         <v>562</v>
       </c>
-      <c r="H132" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J132" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="133" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="2" t="s">
-        <v>467</v>
-      </c>
-      <c r="B133" s="2" t="s">
-        <v>551</v>
-      </c>
-      <c r="C133" s="2" t="s">
+      <c r="G134" s="3" t="s">
         <v>563</v>
       </c>
-      <c r="D133" s="2" t="s">
-        <v>563</v>
-      </c>
-      <c r="E133" s="2" t="s">
-        <v>564</v>
-      </c>
-      <c r="F133" s="2" t="s">
-        <v>565</v>
-      </c>
-      <c r="G133" s="3" t="s">
-        <v>566</v>
-      </c>
-      <c r="H133" s="2" t="s">
+      <c r="H134" s="2" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:AC133" xr:uid="{FB13ADFC-DCBE-45B8-93DC-72D8CCE37DD2}"/>
+  <autoFilter ref="B1:AC134" xr:uid="{FB13ADFC-DCBE-45B8-93DC-72D8CCE37DD2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A46:AC74">
     <sortCondition ref="B2:B132"/>
     <sortCondition ref="N2:N132"/>

</xml_diff>

<commit_message>
update with some english translation
</commit_message>
<xml_diff>
--- a/experimental_context_description.xlsx
+++ b/experimental_context_description.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vignevin-my.sharepoint.com/personal/xavier_delpuech_vignevin_com/Documents/AgricultureNumerique/ProjetsEnCours/VITISDATACROP/05_TRAVAIL_EN_COURS/WP1.1 Harmonisation/Experimentation/vitisdatacrop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="78" documentId="13_ncr:1_{D16C2F42-B43A-4C59-A199-3C52AD3D54E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{212241FC-1091-42E8-8BB4-2BFE6A67AEFA}"/>
+  <xr:revisionPtr revIDLastSave="153" documentId="13_ncr:1_{D16C2F42-B43A-4C59-A199-3C52AD3D54E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1C96E07-6105-48DF-A254-7F5F94CF80F9}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1AE09EEA-C0A3-42DC-AFC7-BA79A75A8C50}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1AE09EEA-C0A3-42DC-AFC7-BA79A75A8C50}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1086" uniqueCount="620">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1143" uniqueCount="677">
   <si>
     <t>experimentation</t>
   </si>
@@ -1904,6 +1904,178 @@
   </si>
   <si>
     <t>link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A description of the file containing the data (dataset), usually in tabular form. The data can be grouped by vintage, stage and/or type according to the desired granularity
+</t>
+  </si>
+  <si>
+    <t>Variable name in data files</t>
+  </si>
+  <si>
+    <t>Description of the variable</t>
+  </si>
+  <si>
+    <t>Data type</t>
+  </si>
+  <si>
+    <t>Characteristic measured</t>
+  </si>
+  <si>
+    <t>Measurement method</t>
+  </si>
+  <si>
+    <t>Data Granularity in data files</t>
+  </si>
+  <si>
+    <t>Unit of the variable</t>
+  </si>
+  <si>
+    <t>Identifier of the variable (typically URI of the Vitis Ontology)</t>
+  </si>
+  <si>
+    <t>Conversion factor to reference variable</t>
+  </si>
+  <si>
+    <t>Brief description of the experimental design. In some cases, there is no experimental design, and if it is a compilation of different studies, it can be specified as "aggregated or reduced data"</t>
+  </si>
+  <si>
+    <t>Type of experimental design according to crop ontology CO_715</t>
+  </si>
+  <si>
+    <t>Number of repetitions for the experimental treatment</t>
+  </si>
+  <si>
+    <t>Year in which the grapes were harvested</t>
+  </si>
+  <si>
+    <t>Experimental Treatment Code</t>
+  </si>
+  <si>
+    <t>The name of the reference variable (standardized name). Use those from the Vitis Ontology.</t>
+  </si>
+  <si>
+    <t>Code of the repetition of the experimental treatment (block, number, etc.)</t>
+  </si>
+  <si>
+    <t>Name (or code) of the field on which the experiment takes place</t>
+  </si>
+  <si>
+    <t>Starting year of the technical itinerary</t>
+  </si>
+  <si>
+    <t>Ending year of the technical itinerary</t>
+  </si>
+  <si>
+    <t>Quantity of water supplied by irrigation over the season, expressed in mm/year. 0 if no irrigation</t>
+  </si>
+  <si>
+    <t>Quantity brought in per ha and per year</t>
+  </si>
+  <si>
+    <t>Form of nitrogen added: mineral or organic</t>
+  </si>
+  <si>
+    <t>Description of the fertilisation usually carried out on the plot</t>
+  </si>
+  <si>
+    <t>Method of supplying fertilising elements</t>
+  </si>
+  <si>
+    <t>Code describing the soil management on the field</t>
+  </si>
+  <si>
+    <t>Type of soil management in the inter-rows</t>
+  </si>
+  <si>
+    <t>Type of soil management under the rows</t>
+  </si>
+  <si>
+    <t>Description of the soil management on the field</t>
+  </si>
+  <si>
+    <t>First and last name of the person</t>
+  </si>
+  <si>
+    <t>Brief description of the observation units</t>
+  </si>
+  <si>
+    <t>Size in m² of experimental units</t>
+  </si>
+  <si>
+    <t>Description of any heterogeneity factors in the experimental design (soil, plant material, topography, etc.)</t>
+  </si>
+  <si>
+    <t>Name of the farm (or estate)</t>
+  </si>
+  <si>
+    <t>Address of the farm</t>
+  </si>
+  <si>
+    <t>Area planted in vines in ha</t>
+  </si>
+  <si>
+    <t>Vineyard number (E.V.V.) commonly known as CVI number (for Casier Viticole Informatisé), with 10 digits</t>
+  </si>
+  <si>
+    <t>Description or comment on the farm</t>
+  </si>
+  <si>
+    <t>SIRET number of the farm</t>
+  </si>
+  <si>
+    <t>Type of event that occurred during the experiment: climatic accident, accident or technical incident, etc.</t>
+  </si>
+  <si>
+    <t>Free description of the event</t>
+  </si>
+  <si>
+    <t>Date (and time) of the event</t>
+  </si>
+  <si>
+    <t>Name or URI of the object(s) impacted by the event (parcel, unit parcel, etc.)</t>
+  </si>
+  <si>
+    <t>Experiment ID (URI or other)</t>
+  </si>
+  <si>
+    <t>Common name (or code) of the experiment</t>
+  </si>
+  <si>
+    <t>Start date of the experiment. It is expressed in the format YYYY-MM-DD according to the international standard ISO 8601.</t>
+  </si>
+  <si>
+    <t>End date of the experiment. It is expressed in the format YYYY-MM-DD according to the international standard ISO 8601.</t>
+  </si>
+  <si>
+    <t>Description of the objectives of the experiment</t>
+  </si>
+  <si>
+    <t>Description of the experiment</t>
+  </si>
+  <si>
+    <t>Acronym of the project(s) associated with the experiment</t>
+  </si>
+  <si>
+    <t>Modality Factor</t>
+  </si>
+  <si>
+    <t>Description of the factor level</t>
+  </si>
+  <si>
+    <t>Code of the factor level</t>
+  </si>
+  <si>
+    <t>Identifier (usually URI) of the factor level</t>
+  </si>
+  <si>
+    <t>Previous cultivation (especially if young vines)</t>
+  </si>
+  <si>
+    <t>Experimental field identifier (URI or other)</t>
+  </si>
+  <si>
+    <t>Brief description or comment on the experimental field</t>
   </si>
 </sst>
 </file>
@@ -2005,7 +2177,7 @@
     <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2042,6 +2214,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -2361,9 +2539,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB13ADFC-DCBE-45B8-93DC-72D8CCE37DD2}">
   <dimension ref="A1:AD127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W89" sqref="W89"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V48" sqref="V48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.85546875" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2376,7 +2554,10 @@
     <col min="6" max="6" width="36.7109375" style="2" customWidth="1"/>
     <col min="7" max="7" width="72" style="2" customWidth="1"/>
     <col min="8" max="8" width="31.85546875" style="2" customWidth="1"/>
-    <col min="9" max="24" width="14.85546875" style="2"/>
+    <col min="9" max="19" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="20" max="21" width="14.85546875" style="2"/>
+    <col min="22" max="22" width="24.42578125" style="15" customWidth="1"/>
+    <col min="23" max="24" width="14.85546875" style="2"/>
     <col min="25" max="25" width="48" style="2" customWidth="1"/>
     <col min="26" max="16384" width="14.85546875" style="2"/>
   </cols>
@@ -2445,7 +2626,7 @@
       <c r="U1" s="1" t="s">
         <v>441</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="14" t="s">
         <v>454</v>
       </c>
       <c r="W1" s="1" t="s">
@@ -2589,6 +2770,9 @@
       <c r="I5" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="V5" s="15" t="s">
+        <v>620</v>
+      </c>
     </row>
     <row r="6" spans="1:30" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -2646,6 +2830,9 @@
       <c r="O7" s="2">
         <v>1</v>
       </c>
+      <c r="V7" s="15" t="s">
+        <v>621</v>
+      </c>
     </row>
     <row r="8" spans="1:30" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -2679,6 +2866,9 @@
       <c r="O8" s="2">
         <v>2</v>
       </c>
+      <c r="V8" s="15" t="s">
+        <v>622</v>
+      </c>
     </row>
     <row r="9" spans="1:30" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -2715,6 +2905,9 @@
       <c r="O9" s="2">
         <v>3</v>
       </c>
+      <c r="V9" s="15" t="s">
+        <v>623</v>
+      </c>
     </row>
     <row r="10" spans="1:30" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -2745,6 +2938,9 @@
       <c r="O10" s="2">
         <v>5</v>
       </c>
+      <c r="V10" s="15" t="s">
+        <v>624</v>
+      </c>
     </row>
     <row r="11" spans="1:30" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -2775,6 +2971,9 @@
       <c r="O11" s="2">
         <v>6</v>
       </c>
+      <c r="V11" s="15" t="s">
+        <v>625</v>
+      </c>
     </row>
     <row r="12" spans="1:30" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
@@ -2808,6 +3007,9 @@
       <c r="O12" s="2">
         <v>7</v>
       </c>
+      <c r="V12" s="15" t="s">
+        <v>626</v>
+      </c>
     </row>
     <row r="13" spans="1:30" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
@@ -2844,6 +3046,9 @@
       <c r="O13" s="2">
         <v>4</v>
       </c>
+      <c r="V13" s="15" t="s">
+        <v>627</v>
+      </c>
     </row>
     <row r="14" spans="1:30" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
@@ -2874,6 +3079,9 @@
       <c r="O14" s="2">
         <v>8</v>
       </c>
+      <c r="V14" s="15" t="s">
+        <v>628</v>
+      </c>
       <c r="Y14" s="7" t="s">
         <v>559</v>
       </c>
@@ -2907,6 +3115,9 @@
       <c r="O15" s="2">
         <v>10</v>
       </c>
+      <c r="V15" s="15" t="s">
+        <v>629</v>
+      </c>
       <c r="Z15" s="2" t="s">
         <v>617</v>
       </c>
@@ -2970,6 +3181,9 @@
       <c r="P17" s="2">
         <v>1</v>
       </c>
+      <c r="V17" s="15" t="s">
+        <v>630</v>
+      </c>
     </row>
     <row r="18" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
@@ -3006,6 +3220,9 @@
       <c r="P18" s="2">
         <v>1</v>
       </c>
+      <c r="V18" s="15" t="s">
+        <v>631</v>
+      </c>
     </row>
     <row r="19" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
@@ -3039,6 +3256,9 @@
       <c r="O19" s="2">
         <v>4</v>
       </c>
+      <c r="V19" s="15" t="s">
+        <v>632</v>
+      </c>
     </row>
     <row r="20" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
@@ -3069,6 +3289,9 @@
       <c r="O20" s="2">
         <v>3</v>
       </c>
+      <c r="V20" s="15" t="s">
+        <v>651</v>
+      </c>
     </row>
     <row r="21" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
@@ -3099,6 +3322,9 @@
       <c r="O21" s="2">
         <v>4</v>
       </c>
+      <c r="V21" s="15" t="s">
+        <v>650</v>
+      </c>
     </row>
     <row r="22" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
@@ -3129,6 +3355,9 @@
       <c r="O22" s="2">
         <v>5</v>
       </c>
+      <c r="V22" s="15" t="s">
+        <v>652</v>
+      </c>
     </row>
     <row r="23" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
@@ -3159,6 +3388,9 @@
       <c r="O23" s="2">
         <v>1</v>
       </c>
+      <c r="V23" s="15" t="s">
+        <v>653</v>
+      </c>
       <c r="AA23" s="2" t="s">
         <v>242</v>
       </c>
@@ -3192,6 +3424,9 @@
       <c r="O24" s="2">
         <v>2</v>
       </c>
+      <c r="V24" s="15" t="s">
+        <v>654</v>
+      </c>
       <c r="AA24" s="2" t="s">
         <v>242</v>
       </c>
@@ -3228,6 +3463,9 @@
       <c r="Q25" s="2">
         <v>0</v>
       </c>
+      <c r="V25" s="15" t="s">
+        <v>655</v>
+      </c>
       <c r="AA25" s="2" t="s">
         <v>243</v>
       </c>
@@ -3261,6 +3499,9 @@
       <c r="O26" s="2">
         <v>3</v>
       </c>
+      <c r="V26" s="15" t="s">
+        <v>656</v>
+      </c>
       <c r="AA26" s="2" t="s">
         <v>248</v>
       </c>
@@ -3291,6 +3532,9 @@
       <c r="O27" s="2">
         <v>5</v>
       </c>
+      <c r="V27" s="15" t="s">
+        <v>657</v>
+      </c>
       <c r="AA27" s="2" t="s">
         <v>249</v>
       </c>
@@ -3324,6 +3568,9 @@
       <c r="O28" s="2">
         <v>4</v>
       </c>
+      <c r="V28" s="15" t="s">
+        <v>658</v>
+      </c>
     </row>
     <row r="29" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
@@ -3351,6 +3598,9 @@
       <c r="I29" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="V29" s="15" t="s">
+        <v>659</v>
+      </c>
     </row>
     <row r="30" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
@@ -3378,6 +3628,9 @@
       <c r="I30" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="V30" s="15" t="s">
+        <v>660</v>
+      </c>
     </row>
     <row r="31" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
@@ -3411,6 +3664,9 @@
       <c r="T31" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="V31" s="15" t="s">
+        <v>661</v>
+      </c>
     </row>
     <row r="32" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
@@ -3438,6 +3694,9 @@
       <c r="I32" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="V32" s="15" t="s">
+        <v>662</v>
+      </c>
     </row>
     <row r="33" spans="1:30" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
@@ -3469,6 +3728,9 @@
       <c r="O33" s="2">
         <v>1</v>
       </c>
+      <c r="V33" s="15" t="s">
+        <v>663</v>
+      </c>
     </row>
     <row r="34" spans="1:30" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
@@ -3508,6 +3770,9 @@
       <c r="P34" s="2">
         <v>1</v>
       </c>
+      <c r="V34" s="15" t="s">
+        <v>664</v>
+      </c>
       <c r="AA34" s="2" t="s">
         <v>277</v>
       </c>
@@ -3550,6 +3815,9 @@
       <c r="T35" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="V35" s="15" t="s">
+        <v>665</v>
+      </c>
       <c r="AA35" s="2" t="s">
         <v>277</v>
       </c>
@@ -3595,6 +3863,9 @@
       <c r="T36" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="V36" s="15" t="s">
+        <v>666</v>
+      </c>
       <c r="AA36" s="2" t="s">
         <v>277</v>
       </c>
@@ -3637,6 +3908,9 @@
       <c r="P37" s="2">
         <v>1</v>
       </c>
+      <c r="V37" s="15" t="s">
+        <v>667</v>
+      </c>
       <c r="AA37" s="2" t="s">
         <v>278</v>
       </c>
@@ -3673,6 +3947,9 @@
       <c r="O38" s="2">
         <v>6</v>
       </c>
+      <c r="V38" s="15" t="s">
+        <v>668</v>
+      </c>
       <c r="AA38" s="2" t="s">
         <v>277</v>
       </c>
@@ -3706,6 +3983,9 @@
       <c r="O39" s="2">
         <v>7</v>
       </c>
+      <c r="V39" s="15" t="s">
+        <v>669</v>
+      </c>
       <c r="AA39" s="2" t="s">
         <v>277</v>
       </c>
@@ -3742,7 +4022,7 @@
       <c r="O40" s="2">
         <v>8</v>
       </c>
-      <c r="V40" s="2" t="s">
+      <c r="V40" s="15" t="s">
         <v>66</v>
       </c>
       <c r="AA40" s="2" t="s">
@@ -3790,6 +4070,9 @@
       <c r="U41" s="2" t="s">
         <v>304</v>
       </c>
+      <c r="V41" s="15" t="s">
+        <v>670</v>
+      </c>
       <c r="AA41" s="2" t="s">
         <v>302</v>
       </c>
@@ -3829,6 +4112,9 @@
       <c r="U42" s="2" t="s">
         <v>303</v>
       </c>
+      <c r="V42" s="15" t="s">
+        <v>672</v>
+      </c>
       <c r="AA42" s="2" t="s">
         <v>302</v>
       </c>
@@ -3865,6 +4151,9 @@
       <c r="P43" s="2">
         <v>1</v>
       </c>
+      <c r="V43" s="15" t="s">
+        <v>671</v>
+      </c>
     </row>
     <row r="44" spans="1:30" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
@@ -3889,6 +4178,9 @@
       <c r="I44" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="V44" s="15" t="s">
+        <v>673</v>
+      </c>
     </row>
     <row r="45" spans="1:30" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
@@ -3925,6 +4217,9 @@
       <c r="P45" s="2">
         <v>2</v>
       </c>
+      <c r="V45" s="15" t="s">
+        <v>675</v>
+      </c>
     </row>
     <row r="46" spans="1:30" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
@@ -3958,6 +4253,9 @@
       <c r="P46" s="2">
         <v>2</v>
       </c>
+      <c r="V46" s="15" t="s">
+        <v>674</v>
+      </c>
     </row>
     <row r="47" spans="1:30" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
@@ -3991,6 +4289,9 @@
       <c r="O47" s="2">
         <v>3</v>
       </c>
+      <c r="V47" s="2" t="s">
+        <v>676</v>
+      </c>
       <c r="AA47" s="2" t="s">
         <v>283</v>
       </c>
@@ -5076,6 +5377,9 @@
       <c r="P73" s="2">
         <v>1</v>
       </c>
+      <c r="V73" s="15" t="s">
+        <v>637</v>
+      </c>
       <c r="AA73" s="2" t="s">
         <v>279</v>
       </c>
@@ -5112,6 +5416,9 @@
       <c r="M74" s="2" t="s">
         <v>324</v>
       </c>
+      <c r="V74" s="15" t="s">
+        <v>638</v>
+      </c>
       <c r="AA74" s="2" t="s">
         <v>231</v>
       </c>
@@ -5145,6 +5452,9 @@
       <c r="M75" s="2" t="s">
         <v>324</v>
       </c>
+      <c r="V75" s="15" t="s">
+        <v>639</v>
+      </c>
     </row>
     <row r="76" spans="1:30" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
@@ -5175,6 +5485,9 @@
       <c r="I76" s="2" t="s">
         <v>437</v>
       </c>
+      <c r="V76" s="15" t="s">
+        <v>640</v>
+      </c>
       <c r="AA76" s="2" t="s">
         <v>231</v>
       </c>
@@ -5208,6 +5521,9 @@
       <c r="I77" s="2" t="s">
         <v>437</v>
       </c>
+      <c r="V77" s="15" t="s">
+        <v>641</v>
+      </c>
     </row>
     <row r="78" spans="1:30" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
@@ -5238,6 +5554,9 @@
       <c r="L78" s="2" t="s">
         <v>103</v>
       </c>
+      <c r="V78" s="15" t="s">
+        <v>642</v>
+      </c>
     </row>
     <row r="79" spans="1:30" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
@@ -5268,6 +5587,9 @@
       <c r="I79" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="V79" s="15" t="s">
+        <v>643</v>
+      </c>
       <c r="AA79" s="2" t="s">
         <v>282</v>
       </c>
@@ -5304,6 +5626,9 @@
       <c r="L80" s="2" t="s">
         <v>187</v>
       </c>
+      <c r="V80" s="15" t="s">
+        <v>644</v>
+      </c>
     </row>
     <row r="81" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
@@ -5334,6 +5659,9 @@
       <c r="P81" s="2">
         <v>2</v>
       </c>
+      <c r="V81" s="15" t="s">
+        <v>645</v>
+      </c>
       <c r="Y81" s="7" t="s">
         <v>541</v>
       </c>
@@ -5370,6 +5698,9 @@
       <c r="P82" s="2">
         <v>2</v>
       </c>
+      <c r="V82" s="15" t="s">
+        <v>646</v>
+      </c>
       <c r="AA82" s="2" t="s">
         <v>231</v>
       </c>
@@ -5406,6 +5737,9 @@
       <c r="P83" s="2">
         <v>2</v>
       </c>
+      <c r="V83" s="15" t="s">
+        <v>647</v>
+      </c>
       <c r="AA83" s="2" t="s">
         <v>231</v>
       </c>
@@ -5439,6 +5773,9 @@
       <c r="P84" s="2">
         <v>2</v>
       </c>
+      <c r="V84" s="15" t="s">
+        <v>648</v>
+      </c>
       <c r="AA84" s="2" t="s">
         <v>282</v>
       </c>
@@ -5505,6 +5842,9 @@
       <c r="P86" s="2">
         <v>1</v>
       </c>
+      <c r="V86" s="15" t="s">
+        <v>649</v>
+      </c>
       <c r="AA86" s="2" t="s">
         <v>277</v>
       </c>
@@ -6674,6 +7014,9 @@
       <c r="O120" s="2">
         <v>2</v>
       </c>
+      <c r="V120" s="15" t="s">
+        <v>634</v>
+      </c>
     </row>
     <row r="121" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
@@ -6770,6 +7113,9 @@
       <c r="O123" s="2">
         <v>9</v>
       </c>
+      <c r="V123" s="15" t="s">
+        <v>635</v>
+      </c>
     </row>
     <row r="124" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
@@ -6794,6 +7140,9 @@
       <c r="I124" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="V124" s="15" t="s">
+        <v>636</v>
+      </c>
     </row>
     <row r="125" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
@@ -6820,6 +7169,9 @@
       </c>
       <c r="I125" s="2" t="s">
         <v>5</v>
+      </c>
+      <c r="V125" s="15" t="s">
+        <v>633</v>
       </c>
     </row>
     <row r="126" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>